<commit_message>
[WIP] Military policies (1)
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB346E8-3DBB-4C89-A97E-15F6B92FD024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B497A376-E90A-42F3-B0D7-BA75FABBDCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="原版" sheetId="1" r:id="rId1"/>
@@ -1081,10 +1081,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>所有单位+7战斗力，所有城市+7战斗力，+7远程力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>所有城市+6战斗力，+5远程力</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1282,6 +1278,10 @@
   </si>
   <si>
     <t>人口大于10/15且有祭祀建筑的城市+25%/+50%信仰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有单位+7战斗力，所有城市+6战斗力，+5远程力</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1313,12 +1313,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1335,7 +1341,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1355,6 +1361,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1844,30 +1862,30 @@
       <selection pane="bottomLeft" activeCell="J3" sqref="J3:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="16.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
-    <col min="14" max="14" width="21.25" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.21875" style="1" customWidth="1"/>
     <col min="15" max="16" width="9" style="1"/>
-    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="20.125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.88671875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.109375" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1908,12 +1926,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1924,10 +1942,10 @@
         <v>13</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1937,7 +1955,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1963,7 +1981,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -1983,7 +2001,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -2000,10 +2018,10 @@
         <v>34</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -2017,7 +2035,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>39</v>
       </c>
@@ -2025,7 +2043,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2039,7 +2057,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C11" s="1" t="s">
         <v>45</v>
       </c>
@@ -2047,7 +2065,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
@@ -2070,7 +2088,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
@@ -2081,7 +2099,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
         <v>57</v>
       </c>
@@ -2089,7 +2107,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="E15" s="1" t="s">
         <v>59</v>
       </c>
@@ -2103,7 +2121,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="E16" s="1" t="s">
         <v>63</v>
       </c>
@@ -2117,7 +2135,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="E17" s="1" t="s">
         <v>66</v>
       </c>
@@ -2129,7 +2147,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
         <v>68</v>
       </c>
@@ -2140,7 +2158,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>71</v>
       </c>
@@ -2148,7 +2166,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="G20" s="1" t="s">
         <v>73</v>
       </c>
@@ -2156,7 +2174,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="I21" s="1" t="s">
         <v>75</v>
       </c>
@@ -2164,7 +2182,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="I22" s="1" t="s">
         <v>77</v>
       </c>
@@ -2181,7 +2199,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="K23" s="1" t="s">
         <v>82</v>
       </c>
@@ -2189,7 +2207,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="M24" s="1" t="s">
         <v>84</v>
       </c>
@@ -2197,7 +2215,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="54" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
       <c r="O25" s="1" t="s">
         <v>86</v>
       </c>
@@ -2205,7 +2223,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="M26" s="1" t="s">
         <v>88</v>
       </c>
@@ -2213,12 +2231,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>91</v>
       </c>
@@ -2232,7 +2250,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:19" ht="72" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>95</v>
       </c>
@@ -2249,7 +2267,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:19" ht="86.4" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>100</v>
       </c>
@@ -2269,7 +2287,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>106</v>
       </c>
@@ -2289,7 +2307,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>112</v>
       </c>
@@ -2309,7 +2327,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
         <v>118</v>
       </c>
@@ -2323,7 +2341,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C35" s="1" t="s">
         <v>121</v>
       </c>
@@ -2335,7 +2353,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C36" s="5" t="s">
         <v>123</v>
       </c>
@@ -2355,7 +2373,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="G37" s="1" t="s">
@@ -2367,7 +2385,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>131</v>
       </c>
@@ -2381,7 +2399,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>135</v>
       </c>
@@ -2395,7 +2413,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="E40" s="1" t="s">
         <v>138</v>
       </c>
@@ -2407,7 +2425,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E41" s="1" t="s">
         <v>140</v>
       </c>
@@ -2421,7 +2439,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="E42" s="1" t="s">
         <v>144</v>
       </c>
@@ -2435,7 +2453,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E43" s="1" t="s">
         <v>148</v>
       </c>
@@ -2443,7 +2461,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="54" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:19" ht="72" x14ac:dyDescent="0.25">
       <c r="E44" s="1" t="s">
         <v>150</v>
       </c>
@@ -2451,7 +2469,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="E45" s="1" t="s">
         <v>152</v>
       </c>
@@ -2459,7 +2477,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:19" ht="72" x14ac:dyDescent="0.25">
       <c r="G46" s="1" t="s">
         <v>154</v>
       </c>
@@ -2470,7 +2488,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="54" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
       <c r="I47" s="1" t="s">
         <v>157</v>
       </c>
@@ -2478,7 +2496,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="I48" s="1" t="s">
         <v>159</v>
       </c>
@@ -2486,7 +2504,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="K49" s="1" t="s">
         <v>161</v>
       </c>
@@ -2494,7 +2512,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="K50" s="1" t="s">
         <v>163</v>
       </c>
@@ -2502,7 +2520,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="M51" s="1" t="s">
         <v>165</v>
       </c>
@@ -2510,7 +2528,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="M52" s="1" t="s">
         <v>167</v>
       </c>
@@ -2518,12 +2536,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>170</v>
       </c>
@@ -2537,7 +2555,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>174</v>
       </c>
@@ -2545,7 +2563,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C57" s="1" t="s">
         <v>176</v>
       </c>
@@ -2559,7 +2577,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E58" s="1" t="s">
         <v>180</v>
       </c>
@@ -2567,7 +2585,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="G59" s="1" t="s">
         <v>182</v>
       </c>
@@ -2575,7 +2593,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="54" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="G60" s="1" t="s">
         <v>184</v>
       </c>
@@ -2583,7 +2601,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="81" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:16" ht="86.4" x14ac:dyDescent="0.25">
       <c r="G61" s="1" t="s">
         <v>186</v>
       </c>
@@ -2591,7 +2609,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="I62" s="1" t="s">
         <v>188</v>
       </c>
@@ -2599,7 +2617,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="54" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="I63" s="1" t="s">
         <v>190</v>
       </c>
@@ -2607,7 +2625,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="K64" s="1" t="s">
         <v>192</v>
       </c>
@@ -2615,7 +2633,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="54" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
       <c r="M65" s="1" t="s">
         <v>193</v>
       </c>
@@ -2623,7 +2641,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="M66" s="1" t="s">
         <v>195</v>
       </c>
@@ -2631,7 +2649,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="94.5" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:19" ht="100.8" x14ac:dyDescent="0.25">
       <c r="O67" s="1" t="s">
         <v>197</v>
       </c>
@@ -2639,7 +2657,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:19" ht="72" x14ac:dyDescent="0.25">
       <c r="O68" s="1" t="s">
         <v>199</v>
       </c>
@@ -2647,7 +2665,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:19" ht="72" x14ac:dyDescent="0.25">
       <c r="O69" s="1" t="s">
         <v>201</v>
       </c>
@@ -2655,12 +2673,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="54" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:19" ht="72" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
         <v>204</v>
       </c>
@@ -2674,7 +2692,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:19" ht="72" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
         <v>208</v>
       </c>
@@ -2688,7 +2706,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C74" s="5" t="s">
         <v>212</v>
       </c>
@@ -2702,7 +2720,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="G75" s="1" t="s">
@@ -2712,7 +2730,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C76" s="1" t="s">
         <v>218</v>
       </c>
@@ -2720,7 +2738,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C77" s="1" t="s">
         <v>220</v>
       </c>
@@ -2728,7 +2746,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="81" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:19" ht="100.8" x14ac:dyDescent="0.25">
       <c r="E78" s="1" t="s">
         <v>222</v>
       </c>
@@ -2745,7 +2763,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
       <c r="I79" s="1" t="s">
         <v>227</v>
       </c>
@@ -2753,12 +2771,12 @@
         <v>228</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
       <c r="K82" s="1" t="s">
         <v>230</v>
       </c>
@@ -2766,7 +2784,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
       <c r="K83" s="1" t="s">
         <v>232</v>
       </c>
@@ -2774,7 +2792,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="54" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:18" ht="57.6" x14ac:dyDescent="0.25">
       <c r="K84" s="1" t="s">
         <v>234</v>
       </c>
@@ -2782,12 +2800,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
       <c r="Q87" s="1" t="s">
         <v>237</v>
       </c>
@@ -2795,7 +2813,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
       <c r="Q88" s="1" t="s">
         <v>239</v>
       </c>
@@ -2803,7 +2821,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
       <c r="Q89" s="1" t="s">
         <v>241</v>
       </c>
@@ -2811,7 +2829,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
       <c r="Q90" s="1" t="s">
         <v>243</v>
       </c>
@@ -2819,7 +2837,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:18" ht="72" x14ac:dyDescent="0.25">
       <c r="Q91" s="1" t="s">
         <v>245</v>
       </c>
@@ -2827,7 +2845,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:18" ht="86.4" x14ac:dyDescent="0.25">
       <c r="Q92" s="1" t="s">
         <v>247</v>
       </c>
@@ -2835,7 +2853,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:18" ht="28.8" x14ac:dyDescent="0.25">
       <c r="Q93" s="1" t="s">
         <v>249</v>
       </c>
@@ -2843,7 +2861,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:18" ht="28.8" x14ac:dyDescent="0.25">
       <c r="Q94" s="1" t="s">
         <v>251</v>
       </c>
@@ -2853,11 +2871,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="C36:C37"/>
@@ -2868,11 +2886,11 @@
     <mergeCell ref="I34:I35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D74:D75"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2884,35 +2902,35 @@
   <dimension ref="A1:U93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T94" sqref="S94:T94"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J95" sqref="J95"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.75" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="16.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" style="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
-    <col min="14" max="14" width="21.25" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.21875" style="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="1"/>
-    <col min="16" max="16" width="16.875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23.875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="20.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.88671875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.77734375" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.88671875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.109375" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2953,29 +2971,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="Q3" s="5" t="s">
+      <c r="J3" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q3" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="R3" s="6" t="s">
-        <v>343</v>
+      <c r="R3" s="8" t="s">
+        <v>393</v>
       </c>
       <c r="T3" s="6" t="s">
         <v>314</v>
@@ -2984,77 +3002,83 @@
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="E4" s="1" t="s">
+    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="E4" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
       <c r="T4" s="5"/>
       <c r="U4" s="6"/>
     </row>
-    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="C5" s="1" t="s">
+    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="C5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="L5" s="6" t="s">
-        <v>344</v>
-      </c>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
+      <c r="L5" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
       <c r="T5" s="1" t="s">
         <v>258</v>
       </c>
       <c r="U5" s="6"/>
     </row>
-    <row r="6" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="C6" s="1" t="s">
+    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
       <c r="T6" s="1" t="s">
         <v>259</v>
       </c>
       <c r="U6" s="6"/>
     </row>
-    <row r="7" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A7" s="1" t="s">
+    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="9" t="s">
         <v>23</v>
       </c>
       <c r="Q7" s="5" t="s">
@@ -3068,23 +3092,31 @@
       </c>
       <c r="U7" s="6"/>
     </row>
-    <row r="8" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A8" s="1" t="s">
+    <row r="8" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="9" t="s">
         <v>29</v>
       </c>
       <c r="Q8" s="5"/>
@@ -3092,35 +3124,55 @@
       <c r="T8" s="5"/>
       <c r="U8" s="6"/>
     </row>
-    <row r="9" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>374</v>
-      </c>
+      <c r="L9" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
       <c r="T9" s="5"/>
       <c r="U9" s="6"/>
     </row>
-    <row r="10" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="M10" s="1" t="s">
+    <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="9" t="s">
         <v>85</v>
       </c>
       <c r="O10" s="1" t="s">
@@ -3136,13 +3188,25 @@
       </c>
       <c r="U10" s="6"/>
     </row>
-    <row r="11" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="G11" s="1" t="s">
+    <row r="11" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="9" t="s">
         <v>74</v>
       </c>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="5"/>
       <c r="T11" s="1" t="s">
@@ -3150,17 +3214,25 @@
       </c>
       <c r="U11" s="6"/>
     </row>
-    <row r="12" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="C12" s="1" t="s">
+    <row r="12" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="9" t="s">
         <v>44</v>
       </c>
       <c r="T12" s="1" t="s">
@@ -3168,25 +3240,45 @@
       </c>
       <c r="U12" s="6"/>
     </row>
-    <row r="13" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="I13" s="1" t="s">
+    <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="9" t="s">
         <v>76</v>
       </c>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
       <c r="T13" s="1" t="s">
         <v>256</v>
       </c>
       <c r="U13" s="6"/>
     </row>
-    <row r="14" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
       <c r="M14" s="1" t="s">
         <v>88</v>
       </c>
@@ -3198,19 +3290,27 @@
       </c>
       <c r="U14" s="6"/>
     </row>
-    <row r="15" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="E15" s="1" t="s">
+    <row r="15" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="J15" s="9" t="s">
         <v>64</v>
       </c>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
       <c r="T15" s="5" t="s">
         <v>270</v>
       </c>
@@ -3218,31 +3318,47 @@
         <v>317</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="E16" s="1" t="s">
+    <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I16" s="5"/>
-      <c r="J16" s="1" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="9" t="s">
         <v>67</v>
       </c>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
       <c r="T16" s="5"/>
       <c r="U16" s="6"/>
     </row>
-    <row r="17" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A17" s="1" t="s">
+    <row r="17" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="9" t="s">
         <v>38</v>
       </c>
       <c r="T17" s="1" t="s">
@@ -3250,23 +3366,29 @@
       </c>
       <c r="U17" s="6"/>
     </row>
-    <row r="18" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="C18" s="1" t="s">
+    <row r="18" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="9" t="s">
         <v>52</v>
       </c>
       <c r="S18" s="1" t="s">
@@ -3277,7 +3399,7 @@
       </c>
       <c r="U18" s="6"/>
     </row>
-    <row r="19" spans="1:21" ht="54.95" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:21" ht="54.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E19" s="1" t="s">
         <v>59</v>
       </c>
@@ -3285,20 +3407,20 @@
         <v>342</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L19" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="S19" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="S19" s="3" t="s">
-        <v>378</v>
-      </c>
       <c r="T19" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="U19" s="6"/>
     </row>
-    <row r="20" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
         <v>45</v>
       </c>
@@ -3310,7 +3432,7 @@
       </c>
       <c r="U20" s="6"/>
     </row>
-    <row r="21" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E21" s="1" t="s">
         <v>68</v>
       </c>
@@ -3325,7 +3447,7 @@
       </c>
       <c r="U21" s="6"/>
     </row>
-    <row r="22" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="I22" s="1" t="s">
         <v>77</v>
       </c>
@@ -3336,42 +3458,42 @@
         <v>79</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="Q22" s="1" t="s">
         <v>273</v>
       </c>
       <c r="R22" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="S22" s="3" t="s">
         <v>379</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>380</v>
       </c>
       <c r="T22" s="5" t="s">
         <v>274</v>
       </c>
       <c r="U22" s="6"/>
     </row>
-    <row r="23" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="K23" s="1" t="s">
+    <row r="23" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="K23" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="L23" s="10" t="s">
         <v>339</v>
       </c>
       <c r="T23" s="5"/>
       <c r="U23" s="6"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="9" t="s">
         <v>92</v>
       </c>
       <c r="K26" s="5" t="s">
@@ -3390,11 +3512,11 @@
         <v>322</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A27" s="1" t="s">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="9" t="s">
         <v>96</v>
       </c>
       <c r="K27" s="5"/>
@@ -3403,7 +3525,7 @@
       <c r="T27" s="5"/>
       <c r="U27" s="6"/>
     </row>
-    <row r="28" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="1" t="s">
         <v>93</v>
       </c>
@@ -3415,7 +3537,7 @@
       </c>
       <c r="U28" s="6"/>
     </row>
-    <row r="29" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C29" s="1" t="s">
         <v>131</v>
       </c>
@@ -3431,7 +3553,7 @@
       <c r="T29" s="5"/>
       <c r="U29" s="6"/>
     </row>
-    <row r="30" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C30" s="1" t="s">
         <v>135</v>
       </c>
@@ -3447,7 +3569,7 @@
       <c r="T30" s="5"/>
       <c r="U30" s="6"/>
     </row>
-    <row r="31" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="E31" s="1" t="s">
         <v>138</v>
       </c>
@@ -3461,7 +3583,7 @@
       <c r="T31" s="5"/>
       <c r="U31" s="6"/>
     </row>
-    <row r="32" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E32" s="1" t="s">
         <v>144</v>
       </c>
@@ -3472,22 +3594,22 @@
         <v>146</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="T32" s="5"/>
       <c r="U32" s="6"/>
     </row>
-    <row r="33" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="I33" s="1" t="s">
         <v>159</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="T33" s="5"/>
       <c r="U33" s="6"/>
     </row>
-    <row r="34" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:21" ht="86.4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>100</v>
       </c>
@@ -3511,7 +3633,7 @@
       </c>
       <c r="U34" s="6"/>
     </row>
-    <row r="35" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>106</v>
       </c>
@@ -3535,7 +3657,7 @@
       </c>
       <c r="U35" s="6"/>
     </row>
-    <row r="36" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="K36" s="1" t="s">
         <v>285</v>
       </c>
@@ -3545,7 +3667,7 @@
       <c r="T36" s="5"/>
       <c r="U36" s="6"/>
     </row>
-    <row r="37" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E37" s="1" t="s">
         <v>140</v>
       </c>
@@ -3561,7 +3683,7 @@
       <c r="T37" s="5"/>
       <c r="U37" s="6"/>
     </row>
-    <row r="38" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C38" s="1" t="s">
         <v>118</v>
       </c>
@@ -3579,7 +3701,7 @@
       </c>
       <c r="U38" s="6"/>
     </row>
-    <row r="39" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C39" s="1" t="s">
         <v>121</v>
       </c>
@@ -3593,12 +3715,12 @@
       <c r="T39" s="5"/>
       <c r="U39" s="6"/>
     </row>
-    <row r="40" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="G40" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="T40" s="5" t="s">
         <v>280</v>
@@ -3607,41 +3729,41 @@
         <v>323</v>
       </c>
     </row>
-    <row r="41" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="G41" s="1" t="s">
         <v>154</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="T41" s="5"/>
       <c r="U41" s="5"/>
     </row>
-    <row r="42" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="I42" s="1" t="s">
         <v>157</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="S42" s="4" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="T42" s="5"/>
       <c r="U42" s="5"/>
     </row>
-    <row r="43" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E43" s="1" t="s">
         <v>150</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="S43" s="2"/>
       <c r="T43" s="5"/>
       <c r="U43" s="5"/>
     </row>
-    <row r="44" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>112</v>
       </c>
@@ -3665,7 +3787,7 @@
       </c>
       <c r="U44" s="5"/>
     </row>
-    <row r="45" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
         <v>123</v>
       </c>
@@ -3676,34 +3798,34 @@
         <v>125</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>288</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="T45" s="5" t="s">
         <v>289</v>
       </c>
       <c r="U45" s="5"/>
     </row>
-    <row r="46" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="G46" s="1" t="s">
         <v>129</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
       <c r="T46" s="5"/>
       <c r="U46" s="5"/>
     </row>
-    <row r="47" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E47" s="1" t="s">
         <v>148</v>
       </c>
@@ -3715,7 +3837,7 @@
       </c>
       <c r="U47" s="5"/>
     </row>
-    <row r="48" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="E48" s="1" t="s">
         <v>152</v>
       </c>
@@ -3729,7 +3851,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K49" s="1" t="s">
         <v>163</v>
       </c>
@@ -3743,7 +3865,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="50" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="M50" s="1" t="s">
         <v>165</v>
       </c>
@@ -3753,7 +3875,7 @@
       <c r="T50" s="5"/>
       <c r="U50" s="5"/>
     </row>
-    <row r="51" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="M51" s="1" t="s">
         <v>167</v>
       </c>
@@ -3769,12 +3891,12 @@
       <c r="T51" s="5"/>
       <c r="U51" s="5"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>170</v>
       </c>
@@ -3800,7 +3922,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="E55" s="1" t="s">
         <v>180</v>
       </c>
@@ -3814,7 +3936,7 @@
       </c>
       <c r="U55" s="6"/>
     </row>
-    <row r="56" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:21" ht="86.4" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>174</v>
       </c>
@@ -3836,7 +3958,7 @@
       <c r="T56" s="5"/>
       <c r="U56" s="6"/>
     </row>
-    <row r="57" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="I57" s="1" t="s">
         <v>190</v>
       </c>
@@ -3848,7 +3970,7 @@
       </c>
       <c r="U57" s="6"/>
     </row>
-    <row r="58" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O58" s="1" t="s">
         <v>199</v>
       </c>
@@ -3858,7 +3980,7 @@
       <c r="T58" s="5"/>
       <c r="U58" s="6"/>
     </row>
-    <row r="59" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O59" s="1" t="s">
         <v>201</v>
       </c>
@@ -3868,18 +3990,18 @@
       <c r="T59" s="5"/>
       <c r="U59" s="6"/>
     </row>
-    <row r="60" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C60" s="1" t="s">
         <v>176</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>178</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="T60" s="1" t="s">
         <v>300</v>
@@ -3888,19 +4010,19 @@
         <v>335</v>
       </c>
     </row>
-    <row r="61" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="G61" s="1" t="s">
         <v>182</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="T61" s="5" t="s">
         <v>301</v>
       </c>
       <c r="U61" s="5"/>
     </row>
-    <row r="62" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="I62" s="1" t="s">
         <v>188</v>
       </c>
@@ -3910,7 +4032,7 @@
       <c r="T62" s="5"/>
       <c r="U62" s="5"/>
     </row>
-    <row r="63" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="G63" s="1" t="s">
         <v>184</v>
       </c>
@@ -3930,7 +4052,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="64" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="M64" s="1" t="s">
         <v>193</v>
       </c>
@@ -3942,7 +4064,7 @@
       <c r="T64" s="5"/>
       <c r="U64" s="5"/>
     </row>
-    <row r="65" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="K65" s="1" t="s">
         <v>192</v>
       </c>
@@ -3953,7 +4075,7 @@
       <c r="T65" s="5"/>
       <c r="U65" s="5"/>
     </row>
-    <row r="66" spans="1:21" ht="81" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:21" ht="86.4" x14ac:dyDescent="0.25">
       <c r="G66" s="1" t="s">
         <v>186</v>
       </c>
@@ -3965,7 +4087,7 @@
       </c>
       <c r="U66" s="5"/>
     </row>
-    <row r="67" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="O67" s="1" t="s">
         <v>197</v>
       </c>
@@ -3982,12 +4104,12 @@
         <v>308</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
         <v>204</v>
       </c>
@@ -4001,7 +4123,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C71" s="1" t="s">
         <v>208</v>
       </c>
@@ -4015,7 +4137,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="72" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C72" s="5" t="s">
         <v>212</v>
       </c>
@@ -4031,7 +4153,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
       <c r="G73" s="1" t="s">
@@ -4041,7 +4163,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="C74" s="1" t="s">
         <v>218</v>
       </c>
@@ -4049,7 +4171,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="75" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="C75" s="1" t="s">
         <v>220</v>
       </c>
@@ -4063,7 +4185,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="76" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="E76" s="1" t="s">
         <v>222</v>
       </c>
@@ -4073,7 +4195,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
       <c r="I77" s="1" t="s">
         <v>227</v>
       </c>
@@ -4081,117 +4203,159 @@
         <v>330</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A81" s="3" t="s">
+      <c r="B81" s="3" t="s">
         <v>346</v>
       </c>
-      <c r="B81" s="3" t="s">
+    </row>
+    <row r="82" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="82" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A82" s="3" t="s">
+      <c r="B82" s="3" t="s">
         <v>348</v>
       </c>
-      <c r="B82" s="3" t="s">
+    </row>
+    <row r="83" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="83" spans="1:16" ht="54" x14ac:dyDescent="0.15">
-      <c r="A83" s="3" t="s">
+      <c r="B83" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="B83" s="3" t="s">
+    </row>
+    <row r="84" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="84" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="A84" s="3" t="s">
+      <c r="B84" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="B84" s="3" t="s">
+    </row>
+    <row r="85" spans="1:16" ht="72" x14ac:dyDescent="0.25">
+      <c r="G85" s="3" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="G85" s="3" t="s">
+      <c r="H85" s="3" t="s">
         <v>354</v>
       </c>
-      <c r="H85" s="3" t="s">
+    </row>
+    <row r="86" spans="1:16" ht="72" x14ac:dyDescent="0.25">
+      <c r="G86" s="3" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="86" spans="1:16" ht="54" x14ac:dyDescent="0.15">
-      <c r="G86" s="3" t="s">
+      <c r="H86" s="3" t="s">
         <v>356</v>
       </c>
-      <c r="H86" s="3" t="s">
+    </row>
+    <row r="87" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="I87" s="3" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="I87" s="3" t="s">
+      <c r="J87" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="J87" s="3" t="s">
+    </row>
+    <row r="88" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
+      <c r="I88" s="3" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="88" spans="1:16" ht="54" x14ac:dyDescent="0.15">
-      <c r="I88" s="3" t="s">
+      <c r="J88" s="3" t="s">
         <v>360</v>
       </c>
-      <c r="J88" s="3" t="s">
+    </row>
+    <row r="89" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="M89" s="3" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" ht="27" x14ac:dyDescent="0.15">
-      <c r="M89" s="3" t="s">
+      <c r="N89" s="3" t="s">
         <v>362</v>
       </c>
-      <c r="N89" s="3" t="s">
+    </row>
+    <row r="90" spans="1:16" ht="72" x14ac:dyDescent="0.25">
+      <c r="M90" s="3" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="90" spans="1:16" ht="54" x14ac:dyDescent="0.15">
-      <c r="M90" s="3" t="s">
+      <c r="N90" s="3" t="s">
         <v>364</v>
       </c>
-      <c r="N90" s="3" t="s">
+    </row>
+    <row r="91" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="O91" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="O91" s="3" t="s">
+      <c r="P91" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="P91" s="3" t="s">
+    </row>
+    <row r="92" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="O92" s="3" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="92" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="O92" s="3" t="s">
+      <c r="P92" s="3" t="s">
         <v>368</v>
       </c>
-      <c r="P92" s="3" t="s">
+    </row>
+    <row r="93" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="O93" s="3" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="93" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="O93" s="3" t="s">
+      <c r="P93" s="3" t="s">
         <v>370</v>
-      </c>
-      <c r="P93" s="3" t="s">
-        <v>371</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="U60:U62"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="Q3:Q6"/>
+    <mergeCell ref="Q7:Q11"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="K71:K72"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q63:Q64"/>
+    <mergeCell ref="K75:K76"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="L75:L76"/>
+    <mergeCell ref="R3:R6"/>
+    <mergeCell ref="R7:R11"/>
+    <mergeCell ref="R54:R55"/>
+    <mergeCell ref="R63:R64"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="U54:U59"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="T26:T27"/>
     <mergeCell ref="U63:U66"/>
     <mergeCell ref="T40:T43"/>
     <mergeCell ref="U15:U23"/>
@@ -4208,48 +4372,6 @@
     <mergeCell ref="U26:U39"/>
     <mergeCell ref="U40:U47"/>
     <mergeCell ref="U49:U51"/>
-    <mergeCell ref="U54:U59"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="T7:T9"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="R3:R6"/>
-    <mergeCell ref="R7:R11"/>
-    <mergeCell ref="R54:R55"/>
-    <mergeCell ref="R63:R64"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="K75:K76"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="L75:L76"/>
-    <mergeCell ref="Q7:Q11"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="K71:K72"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q63:Q64"/>
-    <mergeCell ref="U60:U62"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="Q3:Q6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[WIP] Military policies (2)
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E9348C9-6AFD-406A-8AA1-65EB5D5C8BBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCA257F-E0DA-4584-8E9B-5775158E5531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,25 @@
     <sheet name="原版" sheetId="1" r:id="rId1"/>
     <sheet name="计划" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="397">
   <si>
     <t>远古</t>
   </si>
@@ -812,480 +825,489 @@
     <t>单位生产力</t>
   </si>
   <si>
+    <t>核弹维护费和空军产能</t>
+  </si>
+  <si>
+    <t>单位移动力</t>
+  </si>
+  <si>
+    <t>单位维护费</t>
+  </si>
+  <si>
+    <t>劫掠产出</t>
+  </si>
+  <si>
+    <t>区域建筑生产力</t>
+  </si>
+  <si>
+    <t>资源产出</t>
+  </si>
+  <si>
+    <t>升级所需资源</t>
+  </si>
+  <si>
+    <t>工业区相邻</t>
+  </si>
+  <si>
+    <t>军事学院、码头+4科研</t>
+  </si>
+  <si>
+    <t>航天承包商（科技胜利）</t>
+  </si>
+  <si>
+    <t>三级建筑加强</t>
+  </si>
+  <si>
+    <t>第三选择</t>
+  </si>
+  <si>
+    <t>一党专政</t>
+  </si>
+  <si>
+    <t>所有城市+1全产</t>
+  </si>
+  <si>
+    <t>替代掉了没什么卵用的“保卫祖国”政策——它的效果实在是太没用了</t>
+  </si>
+  <si>
+    <t>城市直接产出</t>
+  </si>
+  <si>
+    <t>大城建筑加成</t>
+  </si>
+  <si>
+    <t>新获得的建造者+1建造次数，生产建造者+30%产能</t>
+  </si>
+  <si>
+    <t>新获得的建造者+2建造次数，生产建造者+30%产能。</t>
+  </si>
+  <si>
+    <t>建造者</t>
+  </si>
+  <si>
+    <t>贸易路线</t>
+  </si>
+  <si>
+    <t>集体化</t>
+  </si>
+  <si>
+    <t>奇观产能</t>
+  </si>
+  <si>
+    <t>开拓者和单元格</t>
+  </si>
+  <si>
+    <t>新政</t>
+  </si>
+  <si>
+    <t>大城住房和宜居度</t>
+  </si>
+  <si>
+    <t>总督加成</t>
+  </si>
+  <si>
+    <t>宗教战斗力</t>
+  </si>
+  <si>
+    <t>旅游业绩</t>
+  </si>
+  <si>
+    <t>韩流（文化胜利）</t>
+  </si>
+  <si>
+    <t>对您有贸易路线的文明+200%旅游业绩，您的摇滚乐队可以选择所有类型的升级</t>
+  </si>
+  <si>
+    <t>外交资本（外交胜利？）</t>
+  </si>
+  <si>
+    <t>影响力点数</t>
+  </si>
+  <si>
+    <t>使者加成</t>
+  </si>
+  <si>
+    <t>首个使者双倍。如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。</t>
+  </si>
+  <si>
+    <t>煽动人心（反制外交胜利）</t>
+  </si>
+  <si>
+    <t>总督忠诚度</t>
+  </si>
+  <si>
+    <t>殖民地发展</t>
+  </si>
+  <si>
+    <t>非国家行为者（反制科技胜利）</t>
+  </si>
+  <si>
+    <t>生产间谍+50%生产力，间谍行动需时-25%；敌方间谍在您的领土内行动时下降2级，您的间谍在进行进攻行动时升高1级；您的间谍可以选择所有类型的升级。</t>
+  </si>
+  <si>
+    <t>间谍</t>
+  </si>
+  <si>
+    <t>同盟关系</t>
+  </si>
+  <si>
+    <t>太空旅游（反制文化胜利）</t>
+  </si>
+  <si>
+    <t>摇滚乐队无法进入您的领土，其他文明对您的旅游业绩下降75%</t>
+  </si>
+  <si>
+    <t>反制文胜</t>
+  </si>
+  <si>
+    <t>每个军营建筑+2大将点数。大将军+2移动力</t>
+  </si>
+  <si>
+    <t>每个学院建筑+2大科点数；每个工业区建筑+2大工点数</t>
+  </si>
+  <si>
+    <t>每回合+4大艺点数，每个艺术博物馆+2大艺点数</t>
+  </si>
+  <si>
+    <t>每回合+2大文学家点数，每个露天剧场+2大文点数</t>
+  </si>
+  <si>
+    <t>每个商业中心建筑+2大商点数；每个港口建筑+2海将点数</t>
+  </si>
+  <si>
+    <t>单位战斗力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域地基加成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗加成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>军转民</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建设军营和港口及其建筑+30%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+4外交支持，+100%影响力点数，开放城邦边界。每个使者+2金币，+1科研</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首个使者双倍。如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。成功下降一个文明的外交胜利点数时，返还50%外交支持。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通往盟友或以您为宗主国的城邦的贸易路线为起终点双方+2食物+2产能，同盟点数增长加速25%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爆铺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精铺</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>文胜</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+2大预言家点数，每个神祠+2大预言家点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+2大将军点数，每个军营或马厩+2大将军点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+2大科学家点数，每个图书馆+2大科学家点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+2海军统帅点数，每个灯塔+2海军统帅点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+2大商人点数，每个市场+2大商人点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+4大音点数，每个歌剧院和广播中心+2大音点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>窃取尤里卡而未被发现的间谍获得一个额外的尤里卡</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宗教</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>城邦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>控制的城邦</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>殖民地</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>帝国</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国际贸易路线从终点的每个战略资源额外+1金+2瓶琴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>拥有至少2次升级的总督提供+2宜居度+1住房</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实验室、军事学院和发电厂+2瓶2琴4钱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>奇观旅游业绩翻倍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>音乐巨作的旅游业绩+100%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有驻防城市+1宜居度，+4忠诚度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有城市+6战斗力，+5远程力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑暗时代政策</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>隐修制度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有圣地城市+75%瓶，所有城市-25%琴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>迟暮勇武</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>近战单位+5战斗力，境外无法恢复生命</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宗教裁判</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使徒可用1次数清洗异教，境内宗教战斗力+15，所有城市-25%瓶</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>孤立主义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国内商路+2粮锤，无法训练移民或建立城市</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>私掠许可</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>海军掠袭单位+100%生产速度，+2移动力，掠夺商路收益翻倍，但商路产量-50%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>敛财大亨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有证券交易所的城市+50%金，有工厂的城市+25%金币，所有城市宜居度-2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>精兵战略</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位+100%经验值，维护费+2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>集体主义</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工业区相邻加成翻倍，所有城市+2住房，农田+1食物，伟人获取-50%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>流氓国家</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>核计划加速+50%，无法获得使者</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>权利归花儿</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>摇滚乐队的业绩对所有未宣战的国家叠加，购买和训练摇滚乐队外的所有陆地单位+100%成本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>网络战</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>攻击信息和未来时代单位+10力，但不满不会下降</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>自动化劳力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生产项目+20%产能，但城市-1宜居-5忠诚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>造谣运动</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个广播中心+3外交支持，但-10%瓶琴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有军事学院或码头的城市+8科研，+15%产能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>驻军加成</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生产轻重骑兵单位+50%产能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有2城区的城市+2住房</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剧院相邻加成+100%，广播中心和体育场+1宜居</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有驻防城市+1宜居度，+8忠诚度，厌战积累-25%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>懒得改掉了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有军事学院、码头或宇航中心的城市：+30%科研，+60%产能，+6电</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>就不凭空造铝了</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非首都大陆城市+15%人口增长，+6忠诚度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有总督城市+10%钱鸽，+4忠诚度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每个总督头衔提供2忠诚度，以及5%钱鸽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>体育传媒会干掉大型歌剧。这不正常，得修掉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>社区+1金，迷人额外+3粮+1锤，惊艳再额外+1粮+1锤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有2城区的城市+1宜居度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有2城区的城市+2住房+1宜居，有3城区的城市+4住房+2宜居</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>军事管制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>击败旧时代单位获得等于其战斗力50%的金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人口大于10/15且有公立学校的城市+25%/50%科技值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人口大于10/15且有银行或造船厂的城市+25%/+50%金币</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人口大于10/15且有歌剧院的城市+25%/+50%文化</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>人口大于10/15且有祭祀建筑的城市+25%/+50%信仰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有单位+7战斗力，所有城市+6战斗力，+5远程力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>非首都大陆城市+25%金币，+10%产能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>核装置维护费-50%，建造空中单位和航母+50%产能</t>
-  </si>
-  <si>
-    <t>核弹维护费和空军产能</t>
-  </si>
-  <si>
-    <t>单位移动力</t>
-  </si>
-  <si>
-    <t>单位维护费</t>
-  </si>
-  <si>
-    <t>劫掠产出</t>
-  </si>
-  <si>
-    <t>区域建筑生产力</t>
-  </si>
-  <si>
-    <t>资源产出</t>
-  </si>
-  <si>
-    <t>升级所需资源</t>
-  </si>
-  <si>
-    <t>工业区相邻</t>
-  </si>
-  <si>
-    <t>军事学院、码头+4科研</t>
-  </si>
-  <si>
-    <t>航天承包商（科技胜利）</t>
-  </si>
-  <si>
-    <t>三级建筑加强</t>
-  </si>
-  <si>
-    <t>第三选择</t>
-  </si>
-  <si>
-    <t>一党专政</t>
-  </si>
-  <si>
-    <t>所有城市+1全产</t>
-  </si>
-  <si>
-    <t>替代掉了没什么卵用的“保卫祖国”政策——它的效果实在是太没用了</t>
-  </si>
-  <si>
-    <t>城市直接产出</t>
-  </si>
-  <si>
-    <t>大城建筑加成</t>
-  </si>
-  <si>
-    <t>新获得的建造者+1建造次数，生产建造者+30%产能</t>
-  </si>
-  <si>
-    <t>新获得的建造者+2建造次数，生产建造者+30%产能。</t>
-  </si>
-  <si>
-    <t>建造者</t>
-  </si>
-  <si>
-    <t>贸易路线</t>
-  </si>
-  <si>
-    <t>集体化</t>
-  </si>
-  <si>
-    <t>奇观产能</t>
-  </si>
-  <si>
-    <t>开拓者和单元格</t>
-  </si>
-  <si>
-    <t>新政</t>
-  </si>
-  <si>
-    <t>大城住房和宜居度</t>
-  </si>
-  <si>
-    <t>总督加成</t>
-  </si>
-  <si>
-    <t>宗教战斗力</t>
-  </si>
-  <si>
-    <t>旅游业绩</t>
-  </si>
-  <si>
-    <t>韩流（文化胜利）</t>
-  </si>
-  <si>
-    <t>对您有贸易路线的文明+200%旅游业绩，您的摇滚乐队可以选择所有类型的升级</t>
-  </si>
-  <si>
-    <t>外交资本（外交胜利？）</t>
-  </si>
-  <si>
-    <t>影响力点数</t>
-  </si>
-  <si>
-    <t>使者加成</t>
-  </si>
-  <si>
-    <t>首个使者双倍。如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。</t>
-  </si>
-  <si>
-    <t>煽动人心（反制外交胜利）</t>
-  </si>
-  <si>
-    <t>总督忠诚度</t>
-  </si>
-  <si>
-    <t>殖民地发展</t>
-  </si>
-  <si>
-    <t>非国家行为者（反制科技胜利）</t>
-  </si>
-  <si>
-    <t>生产间谍+50%生产力，间谍行动需时-25%；敌方间谍在您的领土内行动时下降2级，您的间谍在进行进攻行动时升高1级；您的间谍可以选择所有类型的升级。</t>
-  </si>
-  <si>
-    <t>间谍</t>
-  </si>
-  <si>
-    <t>同盟关系</t>
-  </si>
-  <si>
-    <t>太空旅游（反制文化胜利）</t>
-  </si>
-  <si>
-    <t>摇滚乐队无法进入您的领土，其他文明对您的旅游业绩下降75%</t>
-  </si>
-  <si>
-    <t>反制文胜</t>
-  </si>
-  <si>
-    <t>每个军营建筑+2大将点数。大将军+2移动力</t>
-  </si>
-  <si>
-    <t>每个学院建筑+2大科点数；每个工业区建筑+2大工点数</t>
-  </si>
-  <si>
-    <t>每回合+4大艺点数，每个艺术博物馆+2大艺点数</t>
-  </si>
-  <si>
-    <t>每回合+2大文学家点数，每个露天剧场+2大文点数</t>
-  </si>
-  <si>
-    <t>每个商业中心建筑+2大商点数；每个港口建筑+2海将点数</t>
-  </si>
-  <si>
-    <t>单位战斗力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>区域地基加成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>战斗加成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>军转民</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>建设军营和港口及其建筑+30%生产力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合+4外交支持，+100%影响力点数，开放城邦边界。每个使者+2金币，+1科研</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>首个使者双倍。如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。成功下降一个文明的外交胜利点数时，返还50%外交支持。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>通往盟友或以您为宗主国的城邦的贸易路线为起终点双方+2食物+2产能，同盟点数增长加速25%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>爆铺</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>精铺</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>文胜</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合+2大预言家点数，每个神祠+2大预言家点数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合+2大将军点数，每个军营或马厩+2大将军点数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合+2大科学家点数，每个图书馆+2大科学家点数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合+2海军统帅点数，每个灯塔+2海军统帅点数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合+2大商人点数，每个市场+2大商人点数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每回合+4大音点数，每个歌剧院和广播中心+2大音点</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>窃取尤里卡而未被发现的间谍获得一个额外的尤里卡</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宗教</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>城邦</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>控制的城邦</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>殖民地</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>帝国</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>国际贸易路线从终点的每个战略资源额外+1金+2瓶琴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>拥有至少2次升级的总督提供+2宜居度+1住房</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>实验室、军事学院和发电厂+2瓶2琴4钱</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>奇观旅游业绩翻倍</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>音乐巨作的旅游业绩+100%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有驻防城市+1宜居度，+4忠诚度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有城市+6战斗力，+5远程力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑暗时代政策</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>隐修制度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有圣地城市+75%瓶，所有城市-25%琴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>迟暮勇武</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>近战单位+5战斗力，境外无法恢复生命</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>宗教裁判</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使徒可用1次数清洗异教，境内宗教战斗力+15，所有城市-25%瓶</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>孤立主义</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>国内商路+2粮锤，无法训练移民或建立城市</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>私掠许可</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>海军掠袭单位+100%生产速度，+2移动力，掠夺商路收益翻倍，但商路产量-50%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>敛财大亨</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有证券交易所的城市+50%金，有工厂的城市+25%金币，所有城市宜居度-2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>精兵战略</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>单位+100%经验值，维护费+2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>集体主义</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工业区相邻加成翻倍，所有城市+2住房，农田+1食物，伟人获取-50%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>流氓国家</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>核计划加速+50%，无法获得使者</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>权利归花儿</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>摇滚乐队的业绩对所有未宣战的国家叠加，购买和训练摇滚乐队外的所有陆地单位+100%成本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>网络战</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>攻击信息和未来时代单位+10力，但不满不会下降</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>自动化劳力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生产项目+20%产能，但城市-1宜居-5忠诚</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>造谣运动</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每个广播中心+3外交支持，但-10%瓶琴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有军事学院或码头的城市+8科研，+15%产能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>驻军加成</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生产轻重骑兵单位+50%产能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有2城区的城市+2住房</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>剧院相邻加成+100%，广播中心和体育场+1宜居</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有驻防城市+1宜居度，+8忠诚度，厌战积累-25%</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>懒得改掉了</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有军事学院、码头或宇航中心的城市：+30%科研，+60%产能，+6电</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>就不凭空造铝了</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>非首都大陆城市+15%人口增长，+6忠诚度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有总督城市+10%钱鸽，+4忠诚度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>每个总督头衔提供2忠诚度，以及5%钱鸽</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>体育传媒会干掉大型歌剧。这不正常，得修掉</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>社区+1金，迷人额外+3粮+1锤，惊艳再额外+1粮+1锤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有2城区的城市+1宜居度</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有2城区的城市+2住房+1宜居，有3城区的城市+4住房+2宜居</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>军事管制</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>击败旧时代单位获得等于其战斗力50%的金币</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>人口大于10/15且有公立学校的城市+25%/50%科技值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>人口大于10/15且有银行或造船厂的城市+25%/+50%金币</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>人口大于10/15且有歌剧院的城市+25%/+50%文化</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>人口大于10/15且有祭祀建筑的城市+25%/+50%信仰</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>所有单位+7战斗力，所有城市+6战斗力，+5远程力</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>非首都大陆城市+25%金币，+10%产能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>徭役</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>殖民地办公室政策使城市规划政策失效，城市规划政策在理性主义后过时。此处设置必有问题。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1345,7 +1367,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1373,16 +1395,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1868,8 +1884,8 @@
   <dimension ref="A1:S94"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J3" sqref="J3:J4"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -1952,7 +1968,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
@@ -2028,7 +2044,7 @@
         <v>34</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
@@ -2640,7 +2656,7 @@
         <v>192</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
@@ -2881,11 +2897,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D74:D75"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="C36:C37"/>
@@ -2896,11 +2912,11 @@
     <mergeCell ref="I34:I35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2912,8 +2928,8 @@
   <dimension ref="A1:U93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3020,7 +3036,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -3028,17 +3044,17 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="R3" s="9" t="s">
-        <v>393</v>
+      <c r="R3" s="10" t="s">
+        <v>392</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -3062,8 +3078,8 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
       <c r="T4" s="7"/>
       <c r="U4" s="8"/>
     </row>
@@ -3082,18 +3098,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>343</v>
+      <c r="L5" s="10" t="s">
+        <v>342</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
       <c r="T5" s="1" t="s">
         <v>258</v>
       </c>
@@ -3114,14 +3130,14 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
       <c r="T6" s="1" t="s">
         <v>259</v>
       </c>
@@ -3160,10 +3176,10 @@
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="7" t="s">
+      <c r="Q7" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="R7" s="7" t="s">
+      <c r="R7" s="9" t="s">
         <v>261</v>
       </c>
       <c r="T7" s="7" t="s">
@@ -3200,8 +3216,8 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
       <c r="T8" s="7"/>
       <c r="U8" s="8"/>
     </row>
@@ -3228,14 +3244,14 @@
         <v>34</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="7"/>
-      <c r="R9" s="7"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
       <c r="T9" s="7"/>
       <c r="U9" s="8"/>
     </row>
@@ -3258,16 +3274,16 @@
       <c r="N10" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
+      <c r="T10" s="1" t="s">
         <v>263</v>
-      </c>
-      <c r="Q10" s="7"/>
-      <c r="R10" s="7"/>
-      <c r="T10" s="1" t="s">
-        <v>264</v>
       </c>
       <c r="U10" s="8"/>
     </row>
@@ -3292,10 +3308,10 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="7"/>
-      <c r="R11" s="7"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
       <c r="T11" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="U11" s="8"/>
     </row>
@@ -3327,7 +3343,7 @@
       <c r="Q12" s="5"/>
       <c r="R12" s="5"/>
       <c r="T12" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="U12" s="8"/>
     </row>
@@ -3404,7 +3420,7 @@
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="9" t="s">
         <v>65</v>
       </c>
       <c r="J15" s="5" t="s">
@@ -3419,10 +3435,10 @@
       <c r="Q15" s="5"/>
       <c r="R15" s="5"/>
       <c r="T15" s="7" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="U15" s="8" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -3438,7 +3454,7 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="5" t="s">
         <v>67</v>
       </c>
@@ -3481,7 +3497,7 @@
       <c r="Q17" s="5"/>
       <c r="R17" s="5"/>
       <c r="T17" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="U17" s="8"/>
     </row>
@@ -3520,7 +3536,7 @@
         <v>53</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="U18" s="8"/>
     </row>
@@ -3529,19 +3545,19 @@
         <v>59</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L19" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="S19" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="S19" s="3" t="s">
-        <v>377</v>
-      </c>
       <c r="T19" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="U19" s="8"/>
     </row>
@@ -3552,7 +3568,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3569,7 +3585,7 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="T20" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U20" s="8"/>
     </row>
@@ -3599,7 +3615,7 @@
       <c r="Q21" s="5"/>
       <c r="R21" s="5"/>
       <c r="T21" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="U21" s="8"/>
     </row>
@@ -3608,35 +3624,51 @@
         <v>77</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M22" s="1" t="s">
         <v>79</v>
       </c>
       <c r="N22" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="Q22" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="T22" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="R22" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="T22" s="7" t="s">
+      <c r="U22" s="8"/>
+    </row>
+    <row r="23" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="U22" s="8"/>
-    </row>
-    <row r="23" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="K23" s="11" t="s">
-        <v>275</v>
-      </c>
-      <c r="L23" s="12" t="s">
-        <v>339</v>
-      </c>
+      <c r="L23" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
       <c r="T23" s="7"/>
       <c r="U23" s="8"/>
     </row>
@@ -3645,7 +3677,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>91</v>
       </c>
@@ -3653,22 +3685,22 @@
         <v>92</v>
       </c>
       <c r="K26" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="L26" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="L26" s="7" t="s">
+      <c r="S26" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="S26" s="7" t="s">
+      <c r="T26" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="T26" s="7" t="s">
-        <v>279</v>
-      </c>
       <c r="U26" s="8" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="72" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>95</v>
       </c>
@@ -3677,19 +3709,22 @@
       </c>
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
-      <c r="S27" s="7"/>
+      <c r="S27" s="3" t="s">
+        <v>396</v>
+      </c>
       <c r="T27" s="7"/>
       <c r="U27" s="8"/>
     </row>
-    <row r="28" spans="1:21" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E28" s="1" t="s">
+    <row r="28" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="E28" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="1" t="s">
+      <c r="F28" s="5" t="s">
         <v>94</v>
       </c>
+      <c r="S28" s="3"/>
       <c r="T28" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="U28" s="8"/>
     </row>
@@ -3728,7 +3763,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="10" t="s">
+      <c r="K30" s="9" t="s">
         <v>137</v>
       </c>
       <c r="L30" s="5" t="s">
@@ -3750,7 +3785,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="10"/>
+      <c r="K31" s="9"/>
       <c r="L31" s="5" t="s">
         <v>139</v>
       </c>
@@ -3776,7 +3811,7 @@
         <v>146</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="T32" s="7"/>
       <c r="U32" s="8"/>
@@ -3794,7 +3829,7 @@
         <v>159</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="T33" s="7"/>
       <c r="U33" s="8"/>
@@ -3812,7 +3847,7 @@
         <v>102</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -3820,10 +3855,10 @@
         <v>104</v>
       </c>
       <c r="J34" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="T34" s="1" t="s">
         <v>282</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>283</v>
       </c>
       <c r="U34" s="8"/>
     </row>
@@ -3857,7 +3892,7 @@
         <v>111</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="U35" s="8"/>
     </row>
@@ -3873,7 +3908,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>162</v>
@@ -3902,7 +3937,7 @@
         <v>142</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -3924,14 +3959,14 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="9" t="s">
         <v>120</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>119</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U38" s="8"/>
     </row>
@@ -3946,7 +3981,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
-      <c r="I39" s="10"/>
+      <c r="I39" s="9"/>
       <c r="J39" s="5" t="s">
         <v>122</v>
       </c>
@@ -3958,13 +3993,13 @@
         <v>97</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="U40" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -3972,7 +4007,7 @@
         <v>154</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
@@ -3982,10 +4017,10 @@
         <v>157</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="S42" s="4" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="T42" s="7"/>
       <c r="U42" s="7"/>
@@ -3995,15 +4030,15 @@
         <v>150</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="S43" s="2"/>
       <c r="T43" s="7"/>
       <c r="U43" s="7"/>
     </row>
     <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>112</v>
+      <c r="A44" s="6" t="s">
+        <v>395</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>113</v>
@@ -4025,7 +4060,7 @@
         <v>117</v>
       </c>
       <c r="T44" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U44" s="7"/>
     </row>
@@ -4040,16 +4075,16 @@
         <v>125</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K45" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="T45" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>386</v>
-      </c>
-      <c r="T45" s="7" t="s">
-        <v>289</v>
       </c>
       <c r="U45" s="7"/>
     </row>
@@ -4060,7 +4095,7 @@
         <v>129</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
@@ -4072,10 +4107,10 @@
         <v>148</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="T47" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="U47" s="7"/>
     </row>
@@ -4093,10 +4128,10 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="T48" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4110,13 +4145,13 @@
         <v>163</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="U49" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -4124,7 +4159,7 @@
         <v>165</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="T50" s="7"/>
       <c r="U50" s="7"/>
@@ -4137,10 +4172,10 @@
         <v>168</v>
       </c>
       <c r="Q51" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="R51" s="1" t="s">
         <v>293</v>
-      </c>
-      <c r="R51" s="1" t="s">
-        <v>294</v>
       </c>
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
@@ -4172,16 +4207,16 @@
         <v>173</v>
       </c>
       <c r="Q54" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="R54" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="T54" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="R54" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="T54" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="U54" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -4204,7 +4239,7 @@
       <c r="Q55" s="7"/>
       <c r="R55" s="7"/>
       <c r="T55" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="U55" s="8"/>
     </row>
@@ -4229,13 +4264,13 @@
         <v>195</v>
       </c>
       <c r="N56" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q56" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="Q56" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="R56" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="T56" s="7"/>
       <c r="U56" s="8"/>
@@ -4248,7 +4283,7 @@
         <v>191</v>
       </c>
       <c r="T57" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U57" s="8"/>
     </row>
@@ -4277,19 +4312,19 @@
         <v>176</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>178</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="T60" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="U60" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4297,10 +4332,10 @@
         <v>182</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="T61" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="U61" s="7"/>
     </row>
@@ -4309,7 +4344,7 @@
         <v>188</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="T62" s="7"/>
       <c r="U62" s="7"/>
@@ -4328,16 +4363,16 @@
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
       <c r="Q63" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="R63" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="R63" s="7" t="s">
+      <c r="T63" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="T63" s="7" t="s">
-        <v>304</v>
-      </c>
       <c r="U63" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4367,7 +4402,7 @@
         <v>192</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
@@ -4380,10 +4415,10 @@
         <v>186</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="U66" s="7"/>
     </row>
@@ -4395,13 +4430,13 @@
         <v>198</v>
       </c>
       <c r="Q67" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="R67" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="R67" s="1" t="s">
+      <c r="T67" s="1" t="s">
         <v>307</v>
-      </c>
-      <c r="T67" s="1" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
@@ -4414,13 +4449,13 @@
         <v>204</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>206</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4428,13 +4463,13 @@
         <v>208</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K71" s="7" t="s">
         <v>210</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4442,7 +4477,7 @@
         <v>212</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>214</v>
@@ -4460,7 +4495,7 @@
         <v>216</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4468,7 +4503,7 @@
         <v>218</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4476,13 +4511,13 @@
         <v>220</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K75" s="7" t="s">
         <v>224</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4490,7 +4525,7 @@
         <v>222</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
@@ -4500,120 +4535,161 @@
         <v>227</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>345</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="82" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>347</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="83" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>349</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>351</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="G85" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="H85" s="3" t="s">
         <v>353</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="G86" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H86" s="3" t="s">
         <v>355</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>356</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="I87" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="J87" s="3" t="s">
         <v>357</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="I88" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="J88" s="3" t="s">
         <v>359</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="M89" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="N89" s="3" t="s">
         <v>361</v>
-      </c>
-      <c r="N89" s="3" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="M90" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="N90" s="3" t="s">
         <v>363</v>
-      </c>
-      <c r="N90" s="3" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O91" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="P91" s="3" t="s">
         <v>365</v>
-      </c>
-      <c r="P91" s="3" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="92" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O92" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="P92" s="3" t="s">
         <v>367</v>
-      </c>
-      <c r="P92" s="3" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="93" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O93" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="P93" s="3" t="s">
         <v>369</v>
       </c>
-      <c r="P93" s="3" t="s">
-        <v>370</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="58">
+  <mergeCells count="57">
+    <mergeCell ref="U63:U66"/>
+    <mergeCell ref="T40:T43"/>
+    <mergeCell ref="U15:U23"/>
+    <mergeCell ref="U3:U14"/>
+    <mergeCell ref="T61:T62"/>
+    <mergeCell ref="T63:T65"/>
+    <mergeCell ref="T57:T59"/>
+    <mergeCell ref="T28:T33"/>
+    <mergeCell ref="T35:T37"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="T45:T46"/>
+    <mergeCell ref="T49:T51"/>
+    <mergeCell ref="T55:T56"/>
+    <mergeCell ref="U26:U39"/>
+    <mergeCell ref="U40:U47"/>
+    <mergeCell ref="U49:U51"/>
+    <mergeCell ref="U54:U59"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="R3:R6"/>
+    <mergeCell ref="R7:R11"/>
+    <mergeCell ref="R54:R55"/>
+    <mergeCell ref="R63:R64"/>
+    <mergeCell ref="K75:K76"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="L75:L76"/>
+    <mergeCell ref="Q7:Q11"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="K71:K72"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q63:Q64"/>
     <mergeCell ref="U60:U62"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -4630,48 +4706,6 @@
     <mergeCell ref="K30:K31"/>
     <mergeCell ref="K45:K46"/>
     <mergeCell ref="Q3:Q6"/>
-    <mergeCell ref="Q7:Q11"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="K71:K72"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q63:Q64"/>
-    <mergeCell ref="K75:K76"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="L75:L76"/>
-    <mergeCell ref="R3:R6"/>
-    <mergeCell ref="R7:R11"/>
-    <mergeCell ref="R54:R55"/>
-    <mergeCell ref="R63:R64"/>
-    <mergeCell ref="S26:S27"/>
-    <mergeCell ref="U54:U59"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="T7:T9"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="U63:U66"/>
-    <mergeCell ref="T40:T43"/>
-    <mergeCell ref="U15:U23"/>
-    <mergeCell ref="U3:U14"/>
-    <mergeCell ref="T61:T62"/>
-    <mergeCell ref="T63:T65"/>
-    <mergeCell ref="T57:T59"/>
-    <mergeCell ref="T28:T33"/>
-    <mergeCell ref="T35:T37"/>
-    <mergeCell ref="T38:T39"/>
-    <mergeCell ref="T45:T46"/>
-    <mergeCell ref="T49:T51"/>
-    <mergeCell ref="T55:T56"/>
-    <mergeCell ref="U26:U39"/>
-    <mergeCell ref="U40:U47"/>
-    <mergeCell ref="U49:U51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[Test Needed] Military Policies (fin)
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FCA257F-E0DA-4584-8E9B-5775158E5531}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A22839-DEDA-49E1-B80C-C62D272FF0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -849,9 +849,6 @@
     <t>工业区相邻</t>
   </si>
   <si>
-    <t>军事学院、码头+4科研</t>
-  </si>
-  <si>
     <t>航天承包商（科技胜利）</t>
   </si>
   <si>
@@ -1203,10 +1200,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>有军事学院或码头的城市+8科研，+15%产能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>驻军加成</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1308,6 +1301,14 @@
   </si>
   <si>
     <t>殖民地办公室政策使城市规划政策失效，城市规划政策在理性主义后过时。此处设置必有问题。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有军事学院或码头的城市+15%科研</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有军事学院或码头的城市+15%瓶锤</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1395,10 +1396,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1884,7 +1885,7 @@
   <dimension ref="A1:S94"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
@@ -1968,7 +1969,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
@@ -2044,7 +2045,7 @@
         <v>34</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
@@ -2656,7 +2657,7 @@
         <v>192</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
@@ -2897,11 +2898,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="C36:C37"/>
@@ -2912,11 +2913,11 @@
     <mergeCell ref="I34:I35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D74:D75"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2928,8 +2929,8 @@
   <dimension ref="A1:U93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S28" sqref="S28"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R22" sqref="A22:R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3036,7 +3037,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -3044,17 +3045,17 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="9" t="s">
+      <c r="Q3" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="R3" s="10" t="s">
-        <v>392</v>
+      <c r="R3" s="9" t="s">
+        <v>390</v>
       </c>
       <c r="T3" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -3078,8 +3079,8 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
       <c r="T4" s="7"/>
       <c r="U4" s="8"/>
     </row>
@@ -3098,18 +3099,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="L5" s="10" t="s">
-        <v>342</v>
+      <c r="L5" s="9" t="s">
+        <v>341</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
       <c r="T5" s="1" t="s">
         <v>258</v>
       </c>
@@ -3130,14 +3131,14 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="9"/>
-      <c r="R6" s="9"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
       <c r="T6" s="1" t="s">
         <v>259</v>
       </c>
@@ -3176,10 +3177,10 @@
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="9" t="s">
+      <c r="Q7" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="R7" s="9" t="s">
+      <c r="R7" s="10" t="s">
         <v>261</v>
       </c>
       <c r="T7" s="7" t="s">
@@ -3216,8 +3217,8 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="9"/>
-      <c r="R8" s="9"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
       <c r="T8" s="7"/>
       <c r="U8" s="8"/>
     </row>
@@ -3244,14 +3245,14 @@
         <v>34</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="9"/>
-      <c r="R9" s="9"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
       <c r="T9" s="7"/>
       <c r="U9" s="8"/>
     </row>
@@ -3278,10 +3279,10 @@
         <v>86</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="Q10" s="9"/>
-      <c r="R10" s="9"/>
+        <v>392</v>
+      </c>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
       <c r="T10" s="1" t="s">
         <v>263</v>
       </c>
@@ -3308,8 +3309,8 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
       <c r="T11" s="1" t="s">
         <v>264</v>
       </c>
@@ -3420,7 +3421,7 @@
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="10" t="s">
         <v>65</v>
       </c>
       <c r="J15" s="5" t="s">
@@ -3438,7 +3439,7 @@
         <v>269</v>
       </c>
       <c r="U15" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -3454,7 +3455,7 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="9"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="5" t="s">
         <v>67</v>
       </c>
@@ -3541,23 +3542,37 @@
       <c r="U18" s="8"/>
     </row>
     <row r="19" spans="1:21" ht="54.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E19" s="1" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>341</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>375</v>
-      </c>
+      <c r="F19" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+      <c r="K19" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
       <c r="S19" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="U19" s="8"/>
     </row>
@@ -3568,7 +3583,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3620,29 +3635,41 @@
       <c r="U21" s="8"/>
     </row>
     <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="I22" s="1" t="s">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="J22" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5" t="s">
         <v>271</v>
       </c>
-      <c r="M22" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="N22" s="3" t="s">
-        <v>370</v>
-      </c>
-      <c r="Q22" s="1" t="s">
+      <c r="R22" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="T22" s="7" t="s">
         <v>272</v>
-      </c>
-      <c r="R22" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="S22" s="3" t="s">
-        <v>378</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>273</v>
       </c>
       <c r="U22" s="8"/>
     </row>
@@ -3658,10 +3685,10 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -3685,19 +3712,19 @@
         <v>92</v>
       </c>
       <c r="K26" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="L26" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="L26" s="7" t="s">
+      <c r="S26" s="2" t="s">
         <v>276</v>
       </c>
-      <c r="S26" s="2" t="s">
+      <c r="T26" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="T26" s="7" t="s">
-        <v>278</v>
-      </c>
       <c r="U26" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="72" x14ac:dyDescent="0.25">
@@ -3710,7 +3737,7 @@
       <c r="K27" s="7"/>
       <c r="L27" s="7"/>
       <c r="S27" s="3" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="T27" s="7"/>
       <c r="U27" s="8"/>
@@ -3724,7 +3751,7 @@
       </c>
       <c r="S28" s="3"/>
       <c r="T28" s="8" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="U28" s="8"/>
     </row>
@@ -3763,7 +3790,7 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="10" t="s">
         <v>137</v>
       </c>
       <c r="L30" s="5" t="s">
@@ -3785,7 +3812,7 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="9"/>
+      <c r="K31" s="10"/>
       <c r="L31" s="5" t="s">
         <v>139</v>
       </c>
@@ -3811,7 +3838,7 @@
         <v>146</v>
       </c>
       <c r="N32" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="T32" s="7"/>
       <c r="U32" s="8"/>
@@ -3829,7 +3856,7 @@
         <v>159</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="T33" s="7"/>
       <c r="U33" s="8"/>
@@ -3847,7 +3874,7 @@
         <v>102</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -3855,10 +3882,10 @@
         <v>104</v>
       </c>
       <c r="J34" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="T34" s="1" t="s">
         <v>281</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>282</v>
       </c>
       <c r="U34" s="8"/>
     </row>
@@ -3892,7 +3919,7 @@
         <v>111</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="U35" s="8"/>
     </row>
@@ -3908,7 +3935,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>162</v>
@@ -3937,7 +3964,7 @@
         <v>142</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -3959,14 +3986,14 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-      <c r="I38" s="9" t="s">
+      <c r="I38" s="10" t="s">
         <v>120</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>119</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="U38" s="8"/>
     </row>
@@ -3981,7 +4008,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
-      <c r="I39" s="9"/>
+      <c r="I39" s="10"/>
       <c r="J39" s="5" t="s">
         <v>122</v>
       </c>
@@ -3993,13 +4020,13 @@
         <v>97</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="T40" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="U40" s="8" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4007,7 +4034,7 @@
         <v>154</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
@@ -4017,10 +4044,10 @@
         <v>157</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="S42" s="4" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="T42" s="7"/>
       <c r="U42" s="7"/>
@@ -4030,7 +4057,7 @@
         <v>150</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="S43" s="2"/>
       <c r="T43" s="7"/>
@@ -4038,7 +4065,7 @@
     </row>
     <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>113</v>
@@ -4060,7 +4087,7 @@
         <v>117</v>
       </c>
       <c r="T44" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="U44" s="7"/>
     </row>
@@ -4075,16 +4102,16 @@
         <v>125</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="K45" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="T45" s="7" t="s">
         <v>287</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="T45" s="7" t="s">
-        <v>288</v>
       </c>
       <c r="U45" s="7"/>
     </row>
@@ -4095,7 +4122,7 @@
         <v>129</v>
       </c>
       <c r="H46" s="3" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="K46" s="7"/>
       <c r="L46" s="7"/>
@@ -4107,10 +4134,10 @@
         <v>148</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="T47" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="U47" s="7"/>
     </row>
@@ -4128,10 +4155,10 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="T48" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4145,13 +4172,13 @@
         <v>163</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="U49" s="8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -4159,7 +4186,7 @@
         <v>165</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="T50" s="7"/>
       <c r="U50" s="7"/>
@@ -4172,10 +4199,10 @@
         <v>168</v>
       </c>
       <c r="Q51" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="R51" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="R51" s="1" t="s">
-        <v>293</v>
       </c>
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
@@ -4207,16 +4234,16 @@
         <v>173</v>
       </c>
       <c r="Q54" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="R54" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="T54" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="R54" s="8" t="s">
-        <v>318</v>
-      </c>
-      <c r="T54" s="1" t="s">
-        <v>295</v>
-      </c>
       <c r="U54" s="8" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -4239,7 +4266,7 @@
       <c r="Q55" s="7"/>
       <c r="R55" s="7"/>
       <c r="T55" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="U55" s="8"/>
     </row>
@@ -4264,13 +4291,13 @@
         <v>195</v>
       </c>
       <c r="N56" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q56" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="Q56" s="1" t="s">
-        <v>298</v>
-      </c>
       <c r="R56" s="3" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="T56" s="7"/>
       <c r="U56" s="8"/>
@@ -4283,7 +4310,7 @@
         <v>191</v>
       </c>
       <c r="T57" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="U57" s="8"/>
     </row>
@@ -4312,19 +4339,19 @@
         <v>176</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>178</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="T60" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="U60" s="8" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4332,10 +4359,10 @@
         <v>182</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="T61" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="U61" s="7"/>
     </row>
@@ -4344,7 +4371,7 @@
         <v>188</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="T62" s="7"/>
       <c r="U62" s="7"/>
@@ -4363,16 +4390,16 @@
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
       <c r="Q63" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="R63" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="R63" s="7" t="s">
+      <c r="T63" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="T63" s="7" t="s">
-        <v>303</v>
-      </c>
       <c r="U63" s="8" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4402,7 +4429,7 @@
         <v>192</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
@@ -4415,10 +4442,10 @@
         <v>186</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="U66" s="7"/>
     </row>
@@ -4430,13 +4457,13 @@
         <v>198</v>
       </c>
       <c r="Q67" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="R67" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="R67" s="1" t="s">
+      <c r="T67" s="1" t="s">
         <v>306</v>
-      </c>
-      <c r="T67" s="1" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
@@ -4449,13 +4476,13 @@
         <v>204</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>206</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4463,13 +4490,13 @@
         <v>208</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K71" s="7" t="s">
         <v>210</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4477,7 +4504,7 @@
         <v>212</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>214</v>
@@ -4495,7 +4522,7 @@
         <v>216</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4503,7 +4530,7 @@
         <v>218</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4511,13 +4538,13 @@
         <v>220</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="K75" s="7" t="s">
         <v>224</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4525,7 +4552,7 @@
         <v>222</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
@@ -4535,120 +4562,161 @@
         <v>227</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>344</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="82" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="83" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="B84" s="3" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="G85" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="H85" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="G86" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="H86" s="3" t="s">
         <v>354</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="I87" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="J87" s="3" t="s">
         <v>356</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="I88" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="J88" s="3" t="s">
         <v>358</v>
-      </c>
-      <c r="J88" s="3" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="M89" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="N89" s="3" t="s">
         <v>360</v>
-      </c>
-      <c r="N89" s="3" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="M90" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="N90" s="3" t="s">
         <v>362</v>
-      </c>
-      <c r="N90" s="3" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O91" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="P91" s="3" t="s">
         <v>364</v>
-      </c>
-      <c r="P91" s="3" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="92" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O92" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="P92" s="3" t="s">
         <v>366</v>
-      </c>
-      <c r="P92" s="3" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="93" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O93" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="P93" s="3" t="s">
         <v>368</v>
-      </c>
-      <c r="P93" s="3" t="s">
-        <v>369</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="U60:U62"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="Q3:Q6"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="R3:R6"/>
+    <mergeCell ref="R7:R11"/>
+    <mergeCell ref="R54:R55"/>
+    <mergeCell ref="R63:R64"/>
+    <mergeCell ref="K75:K76"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="L75:L76"/>
+    <mergeCell ref="Q7:Q11"/>
+    <mergeCell ref="K71:K72"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q63:Q64"/>
+    <mergeCell ref="U54:U59"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="T26:T27"/>
     <mergeCell ref="U63:U66"/>
     <mergeCell ref="T40:T43"/>
     <mergeCell ref="U15:U23"/>
@@ -4665,47 +4733,6 @@
     <mergeCell ref="U26:U39"/>
     <mergeCell ref="U40:U47"/>
     <mergeCell ref="U49:U51"/>
-    <mergeCell ref="U54:U59"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="T7:T9"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="R3:R6"/>
-    <mergeCell ref="R7:R11"/>
-    <mergeCell ref="R54:R55"/>
-    <mergeCell ref="R63:R64"/>
-    <mergeCell ref="K75:K76"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="L75:L76"/>
-    <mergeCell ref="Q7:Q11"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="K71:K72"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q63:Q64"/>
-    <mergeCell ref="U60:U62"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="Q3:Q6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[Test Needed] Economic Policies
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A22839-DEDA-49E1-B80C-C62D272FF0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4405F3F5-7747-4FC2-9703-A9B381DC77A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="396">
   <si>
     <t>远古</t>
   </si>
@@ -858,12 +858,6 @@
     <t>第三选择</t>
   </si>
   <si>
-    <t>一党专政</t>
-  </si>
-  <si>
-    <t>所有城市+1全产</t>
-  </si>
-  <si>
     <t>替代掉了没什么卵用的“保卫祖国”政策——它的效果实在是太没用了</t>
   </si>
   <si>
@@ -1212,10 +1206,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>剧院相邻加成+100%，广播中心和体育场+1宜居</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>有驻防城市+1宜居度，+8忠诚度，厌战积累-25%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1300,15 +1290,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>殖民地办公室政策使城市规划政策失效，城市规划政策在理性主义后过时。此处设置必有问题。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>有军事学院或码头的城市+15%科研</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>有军事学院或码头的城市+15%瓶锤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>所有城市+1非信仰产出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一党领导</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>剧院相邻加成+100%，广播中心、体育场和水上运动中心+1宜居</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1368,7 +1366,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1396,11 +1394,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1969,7 +1970,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
@@ -2045,7 +2046,7 @@
         <v>34</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
@@ -2657,7 +2658,7 @@
         <v>192</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
@@ -2898,11 +2899,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D74:D75"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="C36:C37"/>
@@ -2913,11 +2914,11 @@
     <mergeCell ref="I34:I35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2929,8 +2930,8 @@
   <dimension ref="A1:U93"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R22" sqref="A22:R22"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N67" sqref="N67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3037,7 +3038,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -3045,17 +3046,17 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="10" t="s">
+      <c r="Q3" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="R3" s="9" t="s">
-        <v>390</v>
+      <c r="R3" s="10" t="s">
+        <v>387</v>
       </c>
       <c r="T3" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="U3" s="8" t="s">
         <v>312</v>
-      </c>
-      <c r="U3" s="8" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -3079,8 +3080,8 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
       <c r="T4" s="7"/>
       <c r="U4" s="8"/>
     </row>
@@ -3099,18 +3100,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="L5" s="9" t="s">
-        <v>341</v>
+      <c r="L5" s="10" t="s">
+        <v>339</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
       <c r="T5" s="1" t="s">
         <v>258</v>
       </c>
@@ -3131,14 +3132,14 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
       <c r="T6" s="1" t="s">
         <v>259</v>
       </c>
@@ -3177,10 +3178,10 @@
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="9" t="s">
         <v>261</v>
       </c>
       <c r="T7" s="7" t="s">
@@ -3217,8 +3218,8 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="10"/>
-      <c r="R8" s="10"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
       <c r="T8" s="7"/>
       <c r="U8" s="8"/>
     </row>
@@ -3245,14 +3246,14 @@
         <v>34</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="10"/>
+      <c r="Q9" s="9"/>
+      <c r="R9" s="9"/>
       <c r="T9" s="7"/>
       <c r="U9" s="8"/>
     </row>
@@ -3279,10 +3280,10 @@
         <v>86</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
+        <v>389</v>
+      </c>
+      <c r="Q10" s="9"/>
+      <c r="R10" s="9"/>
       <c r="T10" s="1" t="s">
         <v>263</v>
       </c>
@@ -3309,8 +3310,8 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
       <c r="T11" s="1" t="s">
         <v>264</v>
       </c>
@@ -3421,7 +3422,7 @@
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="9" t="s">
         <v>65</v>
       </c>
       <c r="J15" s="5" t="s">
@@ -3439,7 +3440,7 @@
         <v>269</v>
       </c>
       <c r="U15" s="8" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -3455,7 +3456,7 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="10"/>
+      <c r="I16" s="9"/>
       <c r="J16" s="5" t="s">
         <v>67</v>
       </c>
@@ -3550,17 +3551,17 @@
         <v>59</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="6" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
@@ -3569,10 +3570,10 @@
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
       <c r="S19" s="3" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="T19" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="U19" s="8"/>
     </row>
@@ -3583,7 +3584,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3647,7 +3648,7 @@
         <v>77</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -3655,7 +3656,7 @@
         <v>79</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -3663,10 +3664,10 @@
         <v>271</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="T22" s="7" t="s">
         <v>272</v>
@@ -3688,7 +3689,7 @@
         <v>273</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -3704,58 +3705,83 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>91</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="K26" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="L26" s="7" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+      <c r="T26" s="7" t="s">
         <v>275</v>
       </c>
-      <c r="S26" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="T26" s="7" t="s">
-        <v>277</v>
-      </c>
       <c r="U26" s="8" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="72" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>95</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="S27" s="3" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="11" t="s">
         <v>394</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>393</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="2" t="s">
+        <v>274</v>
       </c>
       <c r="T27" s="7"/>
       <c r="U27" s="8"/>
     </row>
-    <row r="28" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="E28" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>94</v>
-      </c>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="S28" s="3"/>
       <c r="T28" s="8" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="U28" s="8"/>
     </row>
     <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A29" s="5"/>
+      <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
         <v>131</v>
       </c>
@@ -3774,10 +3800,18 @@
       <c r="L29" s="5" t="s">
         <v>134</v>
       </c>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
       <c r="T29" s="7"/>
       <c r="U29" s="8"/>
     </row>
     <row r="30" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A30" s="5"/>
+      <c r="B30" s="5"/>
       <c r="C30" s="5" t="s">
         <v>135</v>
       </c>
@@ -3790,16 +3824,24 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="10" t="s">
+      <c r="K30" s="9" t="s">
         <v>137</v>
       </c>
       <c r="L30" s="5" t="s">
         <v>136</v>
       </c>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
       <c r="T30" s="7"/>
       <c r="U30" s="8"/>
     </row>
     <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
@@ -3812,14 +3854,22 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="10"/>
+      <c r="K31" s="9"/>
       <c r="L31" s="5" t="s">
         <v>139</v>
       </c>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
       <c r="T31" s="7"/>
       <c r="U31" s="8"/>
     </row>
     <row r="32" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5" t="s">
@@ -3834,12 +3884,16 @@
       <c r="J32" s="5"/>
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
-      <c r="M32" s="1" t="s">
+      <c r="M32" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="N32" s="3" t="s">
-        <v>372</v>
-      </c>
+      <c r="N32" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
       <c r="T32" s="7"/>
       <c r="U32" s="8"/>
     </row>
@@ -3856,7 +3910,7 @@
         <v>159</v>
       </c>
       <c r="J33" s="6" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="T33" s="7"/>
       <c r="U33" s="8"/>
@@ -3874,7 +3928,7 @@
         <v>102</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
@@ -3882,10 +3936,10 @@
         <v>104</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="T34" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="U34" s="8"/>
     </row>
@@ -3919,7 +3973,7 @@
         <v>111</v>
       </c>
       <c r="T35" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="U35" s="8"/>
     </row>
@@ -3935,7 +3989,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="L36" s="5" t="s">
         <v>162</v>
@@ -3964,7 +4018,7 @@
         <v>142</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
@@ -3986,14 +4040,14 @@
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="9" t="s">
         <v>120</v>
       </c>
       <c r="J38" s="5" t="s">
         <v>119</v>
       </c>
       <c r="T38" s="7" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="U38" s="8"/>
     </row>
@@ -4008,7 +4062,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
-      <c r="I39" s="10"/>
+      <c r="I39" s="9"/>
       <c r="J39" s="5" t="s">
         <v>122</v>
       </c>
@@ -4016,56 +4070,72 @@
       <c r="U39" s="8"/>
     </row>
     <row r="40" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="G40" s="1" t="s">
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>386</v>
-      </c>
+      <c r="H40" s="6" t="s">
+        <v>383</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
       <c r="T40" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="U40" s="8" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="G41" s="1" t="s">
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="H41" s="3" t="s">
-        <v>387</v>
-      </c>
+      <c r="H41" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5"/>
       <c r="T41" s="7"/>
       <c r="U41" s="7"/>
     </row>
     <row r="42" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="I42" s="1" t="s">
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="J42" s="3" t="s">
-        <v>388</v>
+      <c r="J42" s="6" t="s">
+        <v>385</v>
       </c>
       <c r="S42" s="4" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="T42" s="7"/>
       <c r="U42" s="7"/>
     </row>
     <row r="43" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="E43" s="1" t="s">
+      <c r="E43" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>389</v>
-      </c>
+      <c r="F43" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
       <c r="S43" s="2"/>
       <c r="T43" s="7"/>
       <c r="U43" s="7"/>
     </row>
     <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="B44" s="5" t="s">
         <v>113</v>
@@ -4087,57 +4157,61 @@
         <v>117</v>
       </c>
       <c r="T44" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="U44" s="7"/>
+    </row>
+    <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="C45" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>369</v>
+      </c>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="K45" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="U44" s="7"/>
-    </row>
-    <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="C45" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>371</v>
-      </c>
-      <c r="K45" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="L45" s="8" t="s">
-        <v>383</v>
+      <c r="L45" s="10" t="s">
+        <v>380</v>
       </c>
       <c r="T45" s="7" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="U45" s="7"/>
     </row>
     <row r="46" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="G46" s="1" t="s">
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="H46" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
+      <c r="H46" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
       <c r="T46" s="7"/>
       <c r="U46" s="7"/>
     </row>
     <row r="47" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="E47" s="1" t="s">
+      <c r="E47" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>336</v>
+      <c r="F47" s="6" t="s">
+        <v>334</v>
       </c>
       <c r="T47" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="U47" s="7"/>
     </row>
@@ -4155,10 +4229,10 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="T48" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -4172,13 +4246,13 @@
         <v>163</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="T49" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="U49" s="8" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
@@ -4186,7 +4260,7 @@
         <v>165</v>
       </c>
       <c r="N50" s="6" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="T50" s="7"/>
       <c r="U50" s="7"/>
@@ -4198,11 +4272,11 @@
       <c r="N51" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="Q51" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="R51" s="1" t="s">
-        <v>292</v>
+      <c r="Q51" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="R51" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="T51" s="7"/>
       <c r="U51" s="7"/>
@@ -4234,16 +4308,16 @@
         <v>173</v>
       </c>
       <c r="Q54" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="R54" s="8" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="T54" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="U54" s="8" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.25">
@@ -4266,7 +4340,7 @@
       <c r="Q55" s="7"/>
       <c r="R55" s="7"/>
       <c r="T55" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="U55" s="8"/>
     </row>
@@ -4291,13 +4365,13 @@
         <v>195</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q56" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="R56" s="3" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="T56" s="7"/>
       <c r="U56" s="8"/>
@@ -4310,7 +4384,7 @@
         <v>191</v>
       </c>
       <c r="T57" s="8" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="U57" s="8"/>
     </row>
@@ -4339,19 +4413,19 @@
         <v>176</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="O60" s="1" t="s">
         <v>178</v>
       </c>
       <c r="P60" s="3" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="T60" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="U60" s="8" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4359,19 +4433,19 @@
         <v>182</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="T61" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="U61" s="7"/>
     </row>
-    <row r="62" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I62" s="1" t="s">
         <v>188</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="T62" s="7"/>
       <c r="U62" s="7"/>
@@ -4390,16 +4464,16 @@
       <c r="M63" s="5"/>
       <c r="N63" s="5"/>
       <c r="Q63" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="R63" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="T63" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="R63" s="7" t="s">
-        <v>301</v>
-      </c>
-      <c r="T63" s="7" t="s">
-        <v>302</v>
-      </c>
       <c r="U63" s="8" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4429,7 +4503,7 @@
         <v>192</v>
       </c>
       <c r="L65" s="3" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="M65" s="5"/>
       <c r="N65" s="5"/>
@@ -4442,10 +4516,10 @@
         <v>186</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="T66" s="2" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="U66" s="7"/>
     </row>
@@ -4457,13 +4531,13 @@
         <v>198</v>
       </c>
       <c r="Q67" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="R67" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="T67" s="1" t="s">
         <v>304</v>
-      </c>
-      <c r="R67" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="T67" s="1" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.25">
@@ -4476,13 +4550,13 @@
         <v>204</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>206</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
@@ -4490,13 +4564,13 @@
         <v>208</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="K71" s="7" t="s">
         <v>210</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4504,7 +4578,7 @@
         <v>212</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>214</v>
@@ -4522,7 +4596,7 @@
         <v>216</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4530,7 +4604,7 @@
         <v>218</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
@@ -4538,13 +4612,13 @@
         <v>220</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="K75" s="7" t="s">
         <v>224</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
@@ -4552,7 +4626,7 @@
         <v>222</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="K76" s="7"/>
       <c r="L76" s="7"/>
@@ -4562,161 +4636,120 @@
         <v>227</v>
       </c>
       <c r="J77" s="3" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="82" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="83" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="G85" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="G86" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="I87" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
       <c r="I88" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="J88" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
       <c r="M89" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="N89" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="72" x14ac:dyDescent="0.25">
       <c r="M90" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="N90" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O91" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="92" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O92" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="93" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
       <c r="O93" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="P93" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="57">
-    <mergeCell ref="U60:U62"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="Q3:Q6"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="R3:R6"/>
-    <mergeCell ref="R7:R11"/>
-    <mergeCell ref="R54:R55"/>
-    <mergeCell ref="R63:R64"/>
-    <mergeCell ref="K75:K76"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="L75:L76"/>
-    <mergeCell ref="Q7:Q11"/>
-    <mergeCell ref="K71:K72"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q63:Q64"/>
-    <mergeCell ref="U54:U59"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="T7:T9"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="T26:T27"/>
+  <mergeCells count="55">
     <mergeCell ref="U63:U66"/>
     <mergeCell ref="T40:T43"/>
     <mergeCell ref="U15:U23"/>
@@ -4733,6 +4766,45 @@
     <mergeCell ref="U26:U39"/>
     <mergeCell ref="U40:U47"/>
     <mergeCell ref="U49:U51"/>
+    <mergeCell ref="U54:U59"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="R3:R6"/>
+    <mergeCell ref="R7:R11"/>
+    <mergeCell ref="R54:R55"/>
+    <mergeCell ref="R63:R64"/>
+    <mergeCell ref="K75:K76"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="L75:L76"/>
+    <mergeCell ref="Q7:Q11"/>
+    <mergeCell ref="K71:K72"/>
+    <mergeCell ref="Q54:Q55"/>
+    <mergeCell ref="Q63:Q64"/>
+    <mergeCell ref="C72:C73"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I38:I39"/>
+    <mergeCell ref="U60:U62"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K30:K31"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="Q3:Q6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[Test Needed] Diplomatic Policies
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Sistine_civ6mod\文档\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210292D0-3214-44B6-902D-1A8488577C81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19EE1E0-7640-49C1-B794-2DA07A5D53FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="原版" sheetId="1" r:id="rId1"/>
@@ -986,10 +986,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>每回合+4外交支持，+100%影响力点数，开放城邦边界。每个使者+2金币，+1科研</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>首个使者双倍。如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。成功下降一个文明的外交胜利点数时，返还50%外交支持。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1295,6 +1291,10 @@
   </si>
   <si>
     <t>剧院相邻加成+100%，广播中心、体育场和水上运动中心+1宜居</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+4外交支持，+4影响力点数，开放城邦边界。每个使者+1瓶琴钱鸽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1385,10 +1385,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1874,34 +1874,34 @@
   <dimension ref="A1:S94"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="S30" sqref="S30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.21875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.375" style="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
-    <col min="14" max="14" width="21.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.25" style="1" customWidth="1"/>
     <col min="15" max="16" width="9" style="1"/>
-    <col min="17" max="17" width="12.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="13.88671875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="20.109375" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
+    <col min="18" max="18" width="13.875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.125" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1942,12 +1942,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1958,10 +1958,10 @@
         <v>13</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1971,7 +1971,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>30</v>
       </c>
@@ -2034,10 +2034,10 @@
         <v>34</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C9" s="1" t="s">
         <v>39</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="C11" s="1" t="s">
         <v>45</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="C12" s="1" t="s">
         <v>47</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="C13" s="1" t="s">
         <v>54</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C14" s="1" t="s">
         <v>57</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="E15" s="1" t="s">
         <v>59</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="E16" s="1" t="s">
         <v>63</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="E17" s="1" t="s">
         <v>66</v>
       </c>
@@ -2163,7 +2163,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="E18" s="1" t="s">
         <v>68</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="E19" s="1" t="s">
         <v>71</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="G20" s="1" t="s">
         <v>73</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="I21" s="1" t="s">
         <v>75</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="I22" s="1" t="s">
         <v>77</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="K23" s="1" t="s">
         <v>82</v>
       </c>
@@ -2223,7 +2223,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="M24" s="1" t="s">
         <v>84</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="54" x14ac:dyDescent="0.15">
       <c r="O25" s="1" t="s">
         <v>86</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="M26" s="1" t="s">
         <v>88</v>
       </c>
@@ -2247,12 +2247,12 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>91</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>95</v>
       </c>
@@ -2283,7 +2283,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="86.4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>100</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>106</v>
       </c>
@@ -2323,7 +2323,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>112</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C34" s="1" t="s">
         <v>118</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C35" s="1" t="s">
         <v>121</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C36" s="8" t="s">
         <v>123</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
       <c r="G37" s="1" t="s">
@@ -2401,7 +2401,7 @@
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C38" s="1" t="s">
         <v>131</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C39" s="1" t="s">
         <v>135</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="E40" s="1" t="s">
         <v>138</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="E41" s="1" t="s">
         <v>140</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="E42" s="1" t="s">
         <v>144</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="E43" s="1" t="s">
         <v>148</v>
       </c>
@@ -2477,7 +2477,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="54" x14ac:dyDescent="0.15">
       <c r="E44" s="1" t="s">
         <v>150</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.15">
       <c r="E45" s="1" t="s">
         <v>152</v>
       </c>
@@ -2493,7 +2493,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
       <c r="G46" s="1" t="s">
         <v>154</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="54" x14ac:dyDescent="0.15">
       <c r="I47" s="1" t="s">
         <v>157</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="I48" s="1" t="s">
         <v>159</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="K49" s="1" t="s">
         <v>161</v>
       </c>
@@ -2528,7 +2528,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="K50" s="1" t="s">
         <v>163</v>
       </c>
@@ -2536,7 +2536,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="M51" s="1" t="s">
         <v>165</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="M52" s="1" t="s">
         <v>167</v>
       </c>
@@ -2552,12 +2552,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A54" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A55" s="1" t="s">
         <v>170</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A56" s="1" t="s">
         <v>174</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="C57" s="1" t="s">
         <v>176</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.15">
       <c r="E58" s="1" t="s">
         <v>180</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="G59" s="1" t="s">
         <v>182</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="G60" s="1" t="s">
         <v>184</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="86.4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="81" x14ac:dyDescent="0.15">
       <c r="G61" s="1" t="s">
         <v>186</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="I62" s="1" t="s">
         <v>188</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="I63" s="1" t="s">
         <v>190</v>
       </c>
@@ -2641,15 +2641,15 @@
         <v>191</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="K64" s="1" t="s">
         <v>192</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="65" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="65" spans="1:19" ht="54" x14ac:dyDescent="0.15">
       <c r="M65" s="1" t="s">
         <v>193</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="M66" s="1" t="s">
         <v>195</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="100.8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" ht="94.5" x14ac:dyDescent="0.15">
       <c r="O67" s="1" t="s">
         <v>197</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="68" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
       <c r="O68" s="1" t="s">
         <v>199</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="69" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
       <c r="O69" s="1" t="s">
         <v>201</v>
       </c>
@@ -2689,12 +2689,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A71" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="72" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:19" ht="54" x14ac:dyDescent="0.15">
       <c r="C72" s="1" t="s">
         <v>204</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="73" spans="1:19" ht="72" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:19" ht="67.5" x14ac:dyDescent="0.15">
       <c r="C73" s="1" t="s">
         <v>208</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="74" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="C74" s="8" t="s">
         <v>212</v>
       </c>
@@ -2736,7 +2736,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="75" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="C75" s="8"/>
       <c r="D75" s="8"/>
       <c r="G75" s="1" t="s">
@@ -2746,7 +2746,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="76" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C76" s="1" t="s">
         <v>218</v>
       </c>
@@ -2754,7 +2754,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="77" spans="1:19" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:19" ht="27" x14ac:dyDescent="0.15">
       <c r="C77" s="1" t="s">
         <v>220</v>
       </c>
@@ -2762,7 +2762,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="78" spans="1:19" ht="100.8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:19" ht="81" x14ac:dyDescent="0.15">
       <c r="E78" s="1" t="s">
         <v>222</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="79" spans="1:19" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:19" ht="40.5" x14ac:dyDescent="0.15">
       <c r="I79" s="1" t="s">
         <v>227</v>
       </c>
@@ -2787,12 +2787,12 @@
         <v>228</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A81" s="1" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="82" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
       <c r="K82" s="1" t="s">
         <v>230</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="83" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
       <c r="K83" s="1" t="s">
         <v>232</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="84" spans="1:18" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" ht="54" x14ac:dyDescent="0.15">
       <c r="K84" s="1" t="s">
         <v>234</v>
       </c>
@@ -2816,12 +2816,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A86" s="1" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="87" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
       <c r="Q87" s="1" t="s">
         <v>237</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="88" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
       <c r="Q88" s="1" t="s">
         <v>239</v>
       </c>
@@ -2837,7 +2837,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="89" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
       <c r="Q89" s="1" t="s">
         <v>241</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="90" spans="1:18" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:18" ht="40.5" x14ac:dyDescent="0.15">
       <c r="Q90" s="1" t="s">
         <v>243</v>
       </c>
@@ -2853,7 +2853,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="91" spans="1:18" ht="72" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:18" ht="67.5" x14ac:dyDescent="0.15">
       <c r="Q91" s="1" t="s">
         <v>245</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="92" spans="1:18" ht="86.4" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:18" ht="67.5" x14ac:dyDescent="0.15">
       <c r="Q92" s="1" t="s">
         <v>247</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="93" spans="1:18" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:18" ht="27" x14ac:dyDescent="0.15">
       <c r="Q93" s="1" t="s">
         <v>249</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="94" spans="1:18" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:18" ht="27" x14ac:dyDescent="0.15">
       <c r="Q94" s="1" t="s">
         <v>251</v>
       </c>
@@ -2887,11 +2887,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D74:D75"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="C36:C37"/>
@@ -2902,11 +2902,11 @@
     <mergeCell ref="I34:I35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2915,38 +2915,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U93"/>
+  <dimension ref="A1:U92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O74" sqref="O74"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P59" sqref="C59:P59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="17.375" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="11" width="9.21875" style="1" customWidth="1"/>
-    <col min="12" max="12" width="16.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.25" style="1" customWidth="1"/>
+    <col min="12" max="12" width="16.375" style="1" customWidth="1"/>
     <col min="13" max="13" width="9" style="1"/>
-    <col min="14" max="14" width="21.21875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="21.25" style="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="1"/>
-    <col min="16" max="16" width="16.88671875" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.77734375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="23.88671875" style="1" customWidth="1"/>
-    <col min="19" max="19" width="20.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.75" style="1" customWidth="1"/>
+    <col min="18" max="18" width="23.875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="20.125" style="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>10</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="Q2" s="5"/>
       <c r="R2" s="5"/>
     </row>
-    <row r="3" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="41.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -3026,7 +3026,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -3034,11 +3034,11 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="R3" s="10" t="s">
-        <v>384</v>
+      <c r="R3" s="11" t="s">
+        <v>383</v>
       </c>
       <c r="T3" s="9" t="s">
         <v>310</v>
@@ -3047,7 +3047,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -3068,12 +3068,12 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
       <c r="T4" s="8"/>
       <c r="U4" s="9"/>
     </row>
-    <row r="5" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5" t="s">
@@ -3088,24 +3088,24 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="11" t="s">
+      <c r="K5" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="L5" s="10" t="s">
-        <v>339</v>
+      <c r="L5" s="11" t="s">
+        <v>338</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
       <c r="T5" s="1" t="s">
         <v>258</v>
       </c>
       <c r="U5" s="9"/>
     </row>
-    <row r="6" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5" t="s">
@@ -3120,20 +3120,20 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="11"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
       <c r="T6" s="1" t="s">
         <v>259</v>
       </c>
       <c r="U6" s="9"/>
     </row>
-    <row r="7" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -3166,10 +3166,10 @@
       </c>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="11" t="s">
+      <c r="Q7" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="R7" s="11" t="s">
+      <c r="R7" s="10" t="s">
         <v>261</v>
       </c>
       <c r="T7" s="8" t="s">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="U7" s="9"/>
     </row>
-    <row r="8" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -3206,12 +3206,12 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
       <c r="T8" s="8"/>
       <c r="U8" s="9"/>
     </row>
-    <row r="9" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
@@ -3234,18 +3234,18 @@
         <v>34</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
       <c r="T9" s="8"/>
       <c r="U9" s="9"/>
     </row>
-    <row r="10" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -3268,16 +3268,16 @@
         <v>86</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
+        <v>385</v>
+      </c>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
       <c r="T10" s="1" t="s">
         <v>263</v>
       </c>
       <c r="U10" s="9"/>
     </row>
-    <row r="11" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -3298,14 +3298,14 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
       <c r="T11" s="1" t="s">
         <v>264</v>
       </c>
       <c r="U11" s="9"/>
     </row>
-    <row r="12" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5" t="s">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="U12" s="9"/>
     </row>
-    <row r="13" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="U13" s="9"/>
     </row>
-    <row r="14" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="U14" s="9"/>
     </row>
-    <row r="15" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
-      <c r="I15" s="11" t="s">
+      <c r="I15" s="10" t="s">
         <v>65</v>
       </c>
       <c r="J15" s="5" t="s">
@@ -3431,7 +3431,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -3444,7 +3444,7 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="11"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="5" t="s">
         <v>67</v>
       </c>
@@ -3459,7 +3459,7 @@
       <c r="T16" s="8"/>
       <c r="U16" s="9"/>
     </row>
-    <row r="17" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>35</v>
       </c>
@@ -3491,7 +3491,7 @@
       </c>
       <c r="U17" s="9"/>
     </row>
-    <row r="18" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5" t="s">
@@ -3530,7 +3530,7 @@
       </c>
       <c r="U18" s="9"/>
     </row>
-    <row r="19" spans="1:21" ht="54.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="54.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -3539,17 +3539,17 @@
         <v>59</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
@@ -3559,11 +3559,11 @@
       <c r="R19" s="5"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="U19" s="9"/>
     </row>
-    <row r="20" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5" t="s">
@@ -3591,7 +3591,7 @@
       </c>
       <c r="U20" s="9"/>
     </row>
-    <row r="21" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -3621,7 +3621,7 @@
       </c>
       <c r="U21" s="9"/>
     </row>
-    <row r="22" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -3634,7 +3634,7 @@
         <v>77</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -3642,7 +3642,7 @@
         <v>79</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -3650,7 +3650,7 @@
         <v>271</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="S22" s="3"/>
       <c r="T22" s="8" t="s">
@@ -3658,7 +3658,7 @@
       </c>
       <c r="U22" s="9"/>
     </row>
-    <row r="23" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A23" s="5"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -3673,7 +3673,7 @@
         <v>273</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -3684,12 +3684,12 @@
       <c r="T23" s="8"/>
       <c r="U23" s="9"/>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
         <v>91</v>
       </c>
@@ -3720,10 +3720,10 @@
         <v>275</v>
       </c>
       <c r="U26" s="9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="54" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
         <v>95</v>
       </c>
@@ -3739,10 +3739,10 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
@@ -3756,21 +3756,46 @@
       <c r="T27" s="8"/>
       <c r="U27" s="9"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="S28" s="3"/>
+    <row r="28" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="L28" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
       <c r="T28" s="9" t="s">
         <v>311</v>
       </c>
       <c r="U28" s="9"/>
     </row>
-    <row r="29" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="5"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -3778,11 +3803,11 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="5" t="s">
-        <v>133</v>
+      <c r="K29" s="10" t="s">
+        <v>137</v>
       </c>
       <c r="L29" s="5" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -3793,26 +3818,24 @@
       <c r="T29" s="8"/>
       <c r="U29" s="9"/>
     </row>
-    <row r="30" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A30" s="5"/>
       <c r="B30" s="5"/>
-      <c r="C30" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="11" t="s">
-        <v>137</v>
-      </c>
+      <c r="K30" s="10"/>
       <c r="L30" s="5" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
@@ -3823,27 +3846,29 @@
       <c r="T30" s="8"/>
       <c r="U30" s="9"/>
     </row>
-    <row r="31" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
       <c r="E31" s="5" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>139</v>
+        <v>145</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>391</v>
+      </c>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
@@ -3851,133 +3876,131 @@
       <c r="T31" s="8"/>
       <c r="U31" s="9"/>
     </row>
-    <row r="32" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
-      <c r="E32" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>145</v>
-      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>392</v>
-      </c>
-      <c r="O32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="5"/>
-      <c r="R32" s="5"/>
+      <c r="I32" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>374</v>
+      </c>
       <c r="T32" s="8"/>
       <c r="U32" s="9"/>
     </row>
-    <row r="33" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+    <row r="33" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>101</v>
+      </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>277</v>
+      </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>375</v>
+        <v>104</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>278</v>
       </c>
       <c r="T33" s="8"/>
       <c r="U33" s="9"/>
     </row>
-    <row r="34" spans="1:21" ht="86.4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>278</v>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>111</v>
       </c>
       <c r="T34" s="1" t="s">
         <v>279</v>
       </c>
       <c r="U34" s="9"/>
     </row>
-    <row r="35" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>107</v>
-      </c>
+    <row r="35" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>109</v>
-      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
+      <c r="K35" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="L35" s="5" t="s">
+        <v>162</v>
+      </c>
       <c r="M35" s="5"/>
       <c r="N35" s="5"/>
-      <c r="O35" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="P35" s="5" t="s">
-        <v>111</v>
-      </c>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
       <c r="T35" s="8" t="s">
         <v>280</v>
       </c>
       <c r="U35" s="9"/>
     </row>
-    <row r="36" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>141</v>
+      </c>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5" t="s">
-        <v>281</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>162</v>
-      </c>
+      <c r="I36" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="J36" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
       <c r="M36" s="5"/>
       <c r="N36" s="5"/>
       <c r="O36" s="5"/>
@@ -3985,79 +4008,65 @@
       <c r="T36" s="8"/>
       <c r="U36" s="9"/>
     </row>
-    <row r="37" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="F37" s="5" t="s">
-        <v>141</v>
-      </c>
+    <row r="37" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="C37" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J37" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
+      <c r="I37" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="T37" s="8"/>
       <c r="U37" s="9"/>
     </row>
-    <row r="38" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="C38" s="5" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-      <c r="I38" s="11" t="s">
-        <v>120</v>
-      </c>
+      <c r="I38" s="10"/>
       <c r="J38" s="5" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="T38" s="8" t="s">
         <v>283</v>
       </c>
       <c r="U38" s="9"/>
     </row>
-    <row r="39" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="C39" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>122</v>
-      </c>
+    <row r="39" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="5" t="s">
-        <v>122</v>
-      </c>
+      <c r="G39" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
       <c r="T39" s="8"/>
       <c r="U39" s="9"/>
     </row>
-    <row r="40" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" ht="54" x14ac:dyDescent="0.15">
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>380</v>
@@ -4068,709 +4077,708 @@
         <v>276</v>
       </c>
       <c r="U40" s="9" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="H41" s="6" t="s">
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J41" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
+      <c r="S41" s="4"/>
       <c r="T41" s="8"/>
       <c r="U41" s="8"/>
     </row>
-    <row r="42" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
+    <row r="42" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="E42" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>382</v>
+      </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
-      <c r="I42" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J42" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="S42" s="4"/>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5"/>
+      <c r="S42" s="2"/>
       <c r="T42" s="8"/>
       <c r="U42" s="8"/>
     </row>
-    <row r="43" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="A43" s="6" t="s">
+        <v>386</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
       <c r="E43" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>383</v>
+        <v>114</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
-      <c r="S43" s="2"/>
+      <c r="I43" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>117</v>
+      </c>
       <c r="T43" s="8"/>
       <c r="U43" s="8"/>
     </row>
-    <row r="44" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A44" s="6" t="s">
-        <v>387</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+    <row r="44" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="C44" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>124</v>
+      </c>
       <c r="E44" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="F44" s="5" t="s">
-        <v>115</v>
+        <v>125</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>368</v>
       </c>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
-      <c r="I44" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J44" s="5" t="s">
-        <v>117</v>
+      <c r="K44" s="10" t="s">
+        <v>284</v>
+      </c>
+      <c r="L44" s="11" t="s">
+        <v>376</v>
       </c>
       <c r="T44" s="1" t="s">
         <v>282</v>
       </c>
       <c r="U44" s="8"/>
     </row>
-    <row r="45" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="C45" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>369</v>
-      </c>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="K45" s="11" t="s">
-        <v>284</v>
-      </c>
-      <c r="L45" s="10" t="s">
-        <v>377</v>
-      </c>
+    <row r="45" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="C45" s="10"/>
+      <c r="D45" s="10"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>375</v>
+      </c>
+      <c r="K45" s="10"/>
+      <c r="L45" s="10"/>
       <c r="T45" s="8" t="s">
         <v>285</v>
       </c>
       <c r="U45" s="8"/>
     </row>
-    <row r="46" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>376</v>
-      </c>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
+    <row r="46" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="E46" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>333</v>
+      </c>
       <c r="T46" s="8"/>
       <c r="U46" s="8"/>
     </row>
-    <row r="47" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.15">
       <c r="E47" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>334</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
       <c r="T47" s="1" t="s">
         <v>286</v>
       </c>
       <c r="U47" s="8"/>
     </row>
-    <row r="48" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="E48" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>153</v>
-      </c>
+    <row r="48" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
       <c r="G48" s="5"/>
       <c r="H48" s="5"/>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
+      <c r="K48" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="L48" s="6" t="s">
+        <v>335</v>
+      </c>
       <c r="T48" s="1" t="s">
         <v>287</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="L49" s="6" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M49" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="N49" s="6" t="s">
         <v>336</v>
       </c>
       <c r="T49" s="8" t="s">
         <v>288</v>
       </c>
       <c r="U49" s="9" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" ht="28.8" x14ac:dyDescent="0.25">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="54" x14ac:dyDescent="0.15">
       <c r="M50" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="N50" s="6" t="s">
-        <v>337</v>
+        <v>167</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q50" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="R50" s="5" t="s">
+        <v>290</v>
       </c>
       <c r="T50" s="8"/>
       <c r="U50" s="8"/>
     </row>
-    <row r="51" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="M51" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="N51" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="Q51" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="R51" s="5" t="s">
-        <v>290</v>
-      </c>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.15">
       <c r="T51" s="8"/>
       <c r="U51" s="8"/>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A52" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="54" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
+    <row r="53" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="A53" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B53" s="5" t="s">
         <v>171</v>
       </c>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5"/>
+      <c r="H53" s="5"/>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="L53" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+      <c r="P53" s="5"/>
+      <c r="Q53" s="10" t="s">
+        <v>291</v>
+      </c>
+      <c r="R53" s="11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>181</v>
+      </c>
       <c r="G54" s="5"/>
       <c r="H54" s="5"/>
       <c r="I54" s="5"/>
       <c r="J54" s="5"/>
-      <c r="K54" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="L54" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q54" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="R54" s="9" t="s">
-        <v>315</v>
-      </c>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
+      <c r="P54" s="5"/>
+      <c r="Q54" s="10"/>
+      <c r="R54" s="10"/>
       <c r="T54" s="1" t="s">
         <v>292</v>
       </c>
       <c r="U54" s="9" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="5"/>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="A55" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>175</v>
+      </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
-      <c r="E55" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="F55" s="5" t="s">
-        <v>181</v>
-      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
       <c r="G55" s="5"/>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
-      <c r="Q55" s="8"/>
-      <c r="R55" s="8"/>
+      <c r="M55" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="N55" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="Q55" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="R55" s="6" t="s">
+        <v>315</v>
+      </c>
       <c r="T55" s="8" t="s">
         <v>293</v>
       </c>
       <c r="U55" s="9"/>
     </row>
-    <row r="56" spans="1:21" ht="86.4" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>175</v>
-      </c>
+    <row r="56" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="A56" s="5"/>
+      <c r="B56" s="5"/>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="5"/>
       <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
+      <c r="I56" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>191</v>
+      </c>
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
-      <c r="M56" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="N56" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="Q56" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="R56" s="3" t="s">
-        <v>316</v>
-      </c>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
+      <c r="P56" s="5"/>
       <c r="T56" s="8"/>
       <c r="U56" s="9"/>
     </row>
-    <row r="57" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="I57" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>191</v>
+    <row r="57" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="O57" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="P57" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="T57" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="U57" s="9"/>
     </row>
-    <row r="58" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="O58" s="5" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="P58" s="5" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="T58" s="8"/>
       <c r="U58" s="9"/>
     </row>
-    <row r="59" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="C59" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
       <c r="O59" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="P59" s="5" t="s">
-        <v>202</v>
+        <v>178</v>
+      </c>
+      <c r="P59" s="6" t="s">
+        <v>373</v>
       </c>
       <c r="T59" s="8"/>
       <c r="U59" s="9"/>
     </row>
-    <row r="60" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="C60" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D60" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="O60" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="P60" s="3" t="s">
-        <v>374</v>
-      </c>
+    <row r="60" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="G60" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H60" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
       <c r="T60" s="1" t="s">
         <v>296</v>
       </c>
       <c r="U60" s="9" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="G61" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>372</v>
-      </c>
+        <v>330</v>
+      </c>
+    </row>
+    <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J61" s="6" t="s">
+        <v>384</v>
+      </c>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
       <c r="T61" s="8" t="s">
         <v>297</v>
       </c>
       <c r="U61" s="8"/>
     </row>
-    <row r="62" spans="1:21" ht="55.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I62" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>385</v>
+    <row r="62" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G62" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="Q62" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="R62" s="10" t="s">
+        <v>299</v>
       </c>
       <c r="T62" s="8"/>
       <c r="U62" s="8"/>
     </row>
-    <row r="63" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="G63" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>185</v>
-      </c>
+    <row r="63" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
       <c r="I63" s="5"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="Q63" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="R63" s="8" t="s">
-        <v>299</v>
-      </c>
+      <c r="M63" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="N63" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q63" s="10"/>
+      <c r="R63" s="10"/>
       <c r="T63" s="8" t="s">
         <v>300</v>
       </c>
       <c r="U63" s="9" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="G64" s="5"/>
       <c r="H64" s="5"/>
       <c r="I64" s="5"/>
       <c r="J64" s="5"/>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="N64" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q64" s="8"/>
-      <c r="R64" s="8"/>
+      <c r="K64" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="L64" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="P64" s="2"/>
       <c r="T64" s="8"/>
       <c r="U64" s="8"/>
     </row>
-    <row r="65" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
+    <row r="65" spans="1:21" ht="81" x14ac:dyDescent="0.15">
+      <c r="G65" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>316</v>
+      </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
-      <c r="K65" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="L65" s="3" t="s">
-        <v>327</v>
-      </c>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="P65" s="2"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
       <c r="T65" s="8"/>
       <c r="U65" s="8"/>
     </row>
-    <row r="66" spans="1:21" ht="86.4" x14ac:dyDescent="0.25">
-      <c r="G66" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="H66" s="3" t="s">
-        <v>317</v>
+    <row r="66" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="O66" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="P66" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q66" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="R66" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="T66" s="2" t="s">
         <v>301</v>
       </c>
       <c r="U66" s="8"/>
     </row>
-    <row r="67" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="O67" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="P67" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q67" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="R67" s="1" t="s">
-        <v>303</v>
-      </c>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.15">
       <c r="T67" s="1" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A68" s="1" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="70" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C69" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" ht="54" x14ac:dyDescent="0.15">
       <c r="C70" s="1" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>322</v>
       </c>
-      <c r="K70" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C71" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D71" s="3" t="s">
+      <c r="K70" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="L70" s="8" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C71" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>320</v>
+      </c>
+      <c r="G71" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="K71" s="8"/>
+      <c r="L71" s="8"/>
+    </row>
+    <row r="72" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="C72" s="8"/>
+      <c r="D72" s="8"/>
+      <c r="G72" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C73" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C74" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>323</v>
       </c>
-      <c r="K71" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="L71" s="8" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="C72" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="G72" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="K72" s="8"/>
-      <c r="L72" s="8"/>
-    </row>
-    <row r="73" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="C73" s="8"/>
-      <c r="D73" s="8"/>
-      <c r="G73" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H73" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="74" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="C74" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="C75" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D75" s="3" t="s">
+      <c r="K74" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="L74" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="75" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="E75" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="F75" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="K75" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="L75" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="76" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="E76" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F76" s="3" t="s">
+      <c r="K75" s="8"/>
+      <c r="L75" s="8"/>
+    </row>
+    <row r="76" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="I76" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="J76" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="K76" s="8"/>
-      <c r="L76" s="8"/>
-    </row>
-    <row r="77" spans="1:21" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="I77" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J77" s="3" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A79" s="3" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="80" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="81" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="B80" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="82" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="83" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>346</v>
-      </c>
-    </row>
-    <row r="84" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="B84" s="3" t="s">
+    </row>
+    <row r="84" spans="1:16" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="G84" s="3" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="85" spans="1:16" ht="72" x14ac:dyDescent="0.25">
+      <c r="H84" s="3" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="G85" s="3" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="86" spans="1:16" ht="72" x14ac:dyDescent="0.25">
-      <c r="G86" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="H86" s="3" t="s">
+    </row>
+    <row r="86" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+      <c r="I86" s="3" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="87" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="J86" s="3" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="I87" s="3" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" ht="57.6" x14ac:dyDescent="0.25">
-      <c r="I88" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="J88" s="3" t="s">
+    </row>
+    <row r="88" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+      <c r="M88" s="3" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="89" spans="1:16" ht="28.8" x14ac:dyDescent="0.25">
+      <c r="N88" s="3" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="M89" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="N89" s="3" t="s">
-        <v>358</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" ht="72" x14ac:dyDescent="0.25">
-      <c r="M90" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="N90" s="3" t="s">
+    </row>
+    <row r="90" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="O90" s="3" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="91" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+      <c r="P90" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="O91" s="3" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="O92" s="3" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="93" spans="1:16" ht="43.2" x14ac:dyDescent="0.25">
-      <c r="O93" s="3" t="s">
         <v>365</v>
-      </c>
-      <c r="P93" s="3" t="s">
-        <v>366</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="U60:U62"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="K30:K31"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="Q3:Q6"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I38:I39"/>
-    <mergeCell ref="R3:R6"/>
-    <mergeCell ref="R7:R11"/>
-    <mergeCell ref="R54:R55"/>
-    <mergeCell ref="R63:R64"/>
-    <mergeCell ref="K75:K76"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="L75:L76"/>
-    <mergeCell ref="Q7:Q11"/>
-    <mergeCell ref="K71:K72"/>
-    <mergeCell ref="Q54:Q55"/>
-    <mergeCell ref="Q63:Q64"/>
-    <mergeCell ref="U54:U59"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="T7:T9"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="T26:T27"/>
     <mergeCell ref="U63:U66"/>
     <mergeCell ref="T40:T43"/>
     <mergeCell ref="U15:U23"/>
@@ -4787,6 +4795,45 @@
     <mergeCell ref="U26:U39"/>
     <mergeCell ref="U40:U47"/>
     <mergeCell ref="U49:U51"/>
+    <mergeCell ref="U54:U59"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="R7:R11"/>
+    <mergeCell ref="R53:R54"/>
+    <mergeCell ref="R62:R63"/>
+    <mergeCell ref="K74:K75"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="L70:L71"/>
+    <mergeCell ref="L74:L75"/>
+    <mergeCell ref="Q7:Q11"/>
+    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="Q53:Q54"/>
+    <mergeCell ref="Q62:Q63"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="U60:U62"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="K44:K45"/>
+    <mergeCell ref="Q3:Q6"/>
+    <mergeCell ref="R3:R6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
[Test Needed] Great People policies
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19EE1E0-7640-49C1-B794-2DA07A5D53FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A46110B-189F-4DA4-B884-4091D6110570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16050" yWindow="2250" windowWidth="19620" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="原版" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="395">
   <si>
     <t>远古</t>
   </si>
@@ -957,9 +957,6 @@
     <t>每个学院建筑+2大科点数；每个工业区建筑+2大工点数</t>
   </si>
   <si>
-    <t>每回合+4大艺点数，每个艺术博物馆+2大艺点数</t>
-  </si>
-  <si>
     <t>每回合+2大文学家点数，每个露天剧场+2大文点数</t>
   </si>
   <si>
@@ -1295,6 +1292,18 @@
   </si>
   <si>
     <t>每回合+4外交支持，+4影响力点数，开放城邦边界。每个使者+1瓶琴钱鸽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>每回合+4大艺点数，每个艺术和考古博物馆+2大艺点数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发明创造</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>统帅制度（Strategos）</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1873,9 +1882,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S30" sqref="S30"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H75" sqref="H75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1958,7 +1967,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
@@ -2034,7 +2043,7 @@
         <v>34</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="27" x14ac:dyDescent="0.15">
@@ -2646,7 +2655,7 @@
         <v>192</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="54" x14ac:dyDescent="0.15">
@@ -2918,8 +2927,8 @@
   <dimension ref="A1:U92"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P59" sqref="C59:P59"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3026,7 +3035,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -3038,13 +3047,13 @@
         <v>255</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="27" x14ac:dyDescent="0.15">
@@ -3092,7 +3101,7 @@
         <v>257</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -3234,7 +3243,7 @@
         <v>34</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
@@ -3268,7 +3277,7 @@
         <v>86</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -3428,7 +3437,7 @@
         <v>269</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="27" x14ac:dyDescent="0.15">
@@ -3539,17 +3548,17 @@
         <v>59</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
@@ -3559,7 +3568,7 @@
       <c r="R19" s="5"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="U19" s="9"/>
     </row>
@@ -3570,7 +3579,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3634,7 +3643,7 @@
         <v>77</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -3642,7 +3651,7 @@
         <v>79</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -3650,7 +3659,7 @@
         <v>271</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="S22" s="3"/>
       <c r="T22" s="8" t="s">
@@ -3673,7 +3682,7 @@
         <v>273</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -3720,7 +3729,7 @@
         <v>275</v>
       </c>
       <c r="U26" s="9" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="54" x14ac:dyDescent="0.15">
@@ -3739,10 +3748,10 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="7" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
@@ -3784,7 +3793,7 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="T28" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="U28" s="9"/>
     </row>
@@ -3867,7 +3876,7 @@
         <v>146</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
@@ -3889,7 +3898,7 @@
         <v>159</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="T32" s="8"/>
       <c r="U32" s="9"/>
@@ -3997,7 +4006,7 @@
         <v>142</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -4055,7 +4064,7 @@
         <v>97</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -4069,7 +4078,7 @@
         <v>154</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -4077,7 +4086,7 @@
         <v>276</v>
       </c>
       <c r="U40" s="9" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
@@ -4089,7 +4098,7 @@
         <v>157</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="S41" s="4"/>
       <c r="T41" s="8"/>
@@ -4100,7 +4109,7 @@
         <v>150</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
@@ -4112,7 +4121,7 @@
     </row>
     <row r="43" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>113</v>
@@ -4147,7 +4156,7 @@
         <v>125</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
@@ -4155,7 +4164,7 @@
         <v>284</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="T44" s="1" t="s">
         <v>282</v>
@@ -4171,7 +4180,7 @@
         <v>129</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
@@ -4185,7 +4194,7 @@
         <v>148</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="T46" s="8"/>
       <c r="U46" s="8"/>
@@ -4219,13 +4228,13 @@
         <v>163</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="T48" s="1" t="s">
         <v>287</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -4233,13 +4242,13 @@
         <v>165</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="T49" s="8" t="s">
         <v>288</v>
       </c>
       <c r="U49" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="54" x14ac:dyDescent="0.15">
@@ -4296,7 +4305,7 @@
         <v>291</v>
       </c>
       <c r="R53" s="11" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="54" spans="1:21" ht="27" x14ac:dyDescent="0.15">
@@ -4326,7 +4335,7 @@
         <v>292</v>
       </c>
       <c r="U54" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="55" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
@@ -4358,7 +4367,7 @@
         <v>295</v>
       </c>
       <c r="R55" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="T55" s="8" t="s">
         <v>293</v>
@@ -4397,7 +4406,7 @@
         <v>200</v>
       </c>
       <c r="T57" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="U57" s="9"/>
     </row>
@@ -4416,7 +4425,7 @@
         <v>176</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
@@ -4432,7 +4441,7 @@
         <v>178</v>
       </c>
       <c r="P59" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="T59" s="8"/>
       <c r="U59" s="9"/>
@@ -4442,7 +4451,7 @@
         <v>182</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
@@ -4452,7 +4461,7 @@
         <v>296</v>
       </c>
       <c r="U60" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.15">
@@ -4462,7 +4471,7 @@
         <v>188</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
@@ -4512,7 +4521,7 @@
         <v>300</v>
       </c>
       <c r="U63" s="9" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
@@ -4524,7 +4533,7 @@
         <v>192</v>
       </c>
       <c r="L64" s="6" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
@@ -4537,7 +4546,7 @@
         <v>186</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
@@ -4575,206 +4584,256 @@
       </c>
     </row>
     <row r="69" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="C69" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D69" s="3" t="s">
+      <c r="C69" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="E69" s="5"/>
+      <c r="F69" s="5"/>
+      <c r="G69" s="5"/>
+      <c r="H69" s="5"/>
+      <c r="I69" s="5"/>
+      <c r="J69" s="5"/>
+      <c r="K69" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="L69" s="5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="70" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C70" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D70" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="K69" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="L69" s="1" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="C70" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="D70" s="3" t="s">
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+      <c r="K70" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="L70" s="10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C71" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5"/>
+      <c r="G71" s="6" t="s">
+        <v>393</v>
+      </c>
+      <c r="H71" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="I71" s="5"/>
+      <c r="J71" s="5"/>
+      <c r="K71" s="10"/>
+      <c r="L71" s="10"/>
+    </row>
+    <row r="72" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5"/>
+      <c r="G72" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="H72" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+    </row>
+    <row r="73" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C73" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="E73" s="5"/>
+      <c r="F73" s="5"/>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
+      <c r="I73" s="5"/>
+      <c r="J73" s="5"/>
+      <c r="K73" s="5"/>
+      <c r="L73" s="5"/>
+    </row>
+    <row r="74" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C74" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D74" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="K70" s="8" t="s">
-        <v>210</v>
-      </c>
-      <c r="L70" s="8" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C71" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="K71" s="8"/>
-      <c r="L71" s="8"/>
-    </row>
-    <row r="72" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
-      <c r="G72" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="C73" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="D73" s="1" t="s">
+      <c r="E74" s="5"/>
+      <c r="F74" s="5"/>
+      <c r="G74" s="5"/>
+      <c r="H74" s="5"/>
+      <c r="I74" s="5"/>
+      <c r="J74" s="5"/>
+      <c r="K74" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="L74" s="10" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="74" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="C74" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="D74" s="3" t="s">
+    <row r="75" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+      <c r="E75" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="F75" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="K74" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="L74" s="8" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="75" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="E75" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="F75" s="3" t="s">
+      <c r="G75" s="5"/>
+      <c r="H75" s="5"/>
+      <c r="I75" s="5"/>
+      <c r="J75" s="5"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+    </row>
+    <row r="76" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+      <c r="E76" s="5"/>
+      <c r="F76" s="5"/>
+      <c r="G76" s="5"/>
+      <c r="H76" s="5"/>
+      <c r="I76" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="J76" s="6" t="s">
         <v>324</v>
       </c>
-      <c r="K75" s="8"/>
-      <c r="L75" s="8"/>
-    </row>
-    <row r="76" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="I76" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="J76" s="3" t="s">
-        <v>325</v>
-      </c>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="80" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B80" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="B80" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B81" s="3" t="s">
         <v>342</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="82" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>344</v>
-      </c>
-      <c r="B82" s="3" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="83" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="B83" s="3" t="s">
         <v>346</v>
-      </c>
-      <c r="B83" s="3" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="67.5" x14ac:dyDescent="0.15">
       <c r="G84" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="H84" s="3" t="s">
         <v>348</v>
-      </c>
-      <c r="H84" s="3" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="G85" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="H85" s="3" t="s">
         <v>350</v>
-      </c>
-      <c r="H85" s="3" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="I86" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="J86" s="3" t="s">
         <v>352</v>
-      </c>
-      <c r="J86" s="3" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="I87" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="J87" s="3" t="s">
         <v>354</v>
-      </c>
-      <c r="J87" s="3" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="M88" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="N88" s="3" t="s">
         <v>356</v>
-      </c>
-      <c r="N88" s="3" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="M89" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="N89" s="3" t="s">
         <v>358</v>
-      </c>
-      <c r="N89" s="3" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="O90" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="P90" s="3" t="s">
         <v>360</v>
-      </c>
-      <c r="P90" s="3" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="O91" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="P91" s="3" t="s">
         <v>362</v>
-      </c>
-      <c r="P91" s="3" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="92" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="O92" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="P92" s="3" t="s">
         <v>364</v>
-      </c>
-      <c r="P92" s="3" t="s">
-        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Short circuit Diplomatic League
To save AI performance
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A46110B-189F-4DA4-B884-4091D6110570}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2746DD-8F0F-4C5D-92A0-60156074BB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16050" yWindow="2250" windowWidth="19620" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="原版" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="396">
   <si>
     <t>远古</t>
   </si>
@@ -918,9 +918,6 @@
     <t>使者加成</t>
   </si>
   <si>
-    <t>首个使者双倍。如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。</t>
-  </si>
-  <si>
     <t>煽动人心（反制外交胜利）</t>
   </si>
   <si>
@@ -983,10 +980,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>首个使者双倍。如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。成功下降一个文明的外交胜利点数时，返还50%外交支持。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>通往盟友或以您为宗主国的城邦的贸易路线为起终点双方+2食物+2产能，同盟点数增长加速25%</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1304,6 +1297,18 @@
   </si>
   <si>
     <t>统帅制度（Strategos）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>如果城邦宗主国和您的政体不同，您派出的使者被视为翻倍。成功下降一个文明的外交胜利点数时，返还50%外交支持。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>首个使者双倍</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1967,7 +1972,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.15">
@@ -2043,7 +2048,7 @@
         <v>34</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="27" x14ac:dyDescent="0.15">
@@ -2655,7 +2660,7 @@
         <v>192</v>
       </c>
       <c r="L64" s="3" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="65" spans="1:19" ht="54" x14ac:dyDescent="0.15">
@@ -2896,11 +2901,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="C36:C37"/>
@@ -2911,11 +2916,11 @@
     <mergeCell ref="I34:I35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D74:D75"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2926,9 +2931,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U92"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3035,7 +3040,7 @@
         <v>13</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
@@ -3047,13 +3052,13 @@
         <v>255</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="U3" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="27" x14ac:dyDescent="0.15">
@@ -3101,7 +3106,7 @@
         <v>257</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -3243,7 +3248,7 @@
         <v>34</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
@@ -3277,7 +3282,7 @@
         <v>86</v>
       </c>
       <c r="P10" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="Q10" s="10"/>
       <c r="R10" s="10"/>
@@ -3437,7 +3442,7 @@
         <v>269</v>
       </c>
       <c r="U15" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="27" x14ac:dyDescent="0.15">
@@ -3548,17 +3553,17 @@
         <v>59</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
       <c r="K19" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="L19" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
@@ -3568,7 +3573,7 @@
       <c r="R19" s="5"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="U19" s="9"/>
     </row>
@@ -3579,7 +3584,7 @@
         <v>45</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -3643,7 +3648,7 @@
         <v>77</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
@@ -3651,7 +3656,7 @@
         <v>79</v>
       </c>
       <c r="N22" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -3659,7 +3664,7 @@
         <v>271</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="S22" s="3"/>
       <c r="T22" s="8" t="s">
@@ -3682,7 +3687,7 @@
         <v>273</v>
       </c>
       <c r="L23" s="6" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="M23" s="5"/>
       <c r="N23" s="5"/>
@@ -3729,7 +3734,7 @@
         <v>275</v>
       </c>
       <c r="U26" s="9" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="54" x14ac:dyDescent="0.15">
@@ -3748,10 +3753,10 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
       <c r="K27" s="7" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="M27" s="5"/>
       <c r="N27" s="5"/>
@@ -3793,7 +3798,7 @@
       <c r="Q28" s="5"/>
       <c r="R28" s="5"/>
       <c r="T28" s="9" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="U28" s="9"/>
     </row>
@@ -3876,7 +3881,7 @@
         <v>146</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="O31" s="5"/>
       <c r="P31" s="5"/>
@@ -3898,7 +3903,7 @@
         <v>159</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="T32" s="8"/>
       <c r="U32" s="9"/>
@@ -4006,7 +4011,7 @@
         <v>142</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
@@ -4064,7 +4069,7 @@
         <v>97</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
@@ -4078,7 +4083,7 @@
         <v>154</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
@@ -4086,7 +4091,7 @@
         <v>276</v>
       </c>
       <c r="U40" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="41" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
@@ -4098,7 +4103,7 @@
         <v>157</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="S41" s="4"/>
       <c r="T41" s="8"/>
@@ -4109,7 +4114,7 @@
         <v>150</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
@@ -4121,7 +4126,7 @@
     </row>
     <row r="43" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A43" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>113</v>
@@ -4156,7 +4161,7 @@
         <v>125</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
@@ -4164,7 +4169,7 @@
         <v>284</v>
       </c>
       <c r="L44" s="11" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="T44" s="1" t="s">
         <v>282</v>
@@ -4180,7 +4185,7 @@
         <v>129</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="K45" s="10"/>
       <c r="L45" s="10"/>
@@ -4194,7 +4199,7 @@
         <v>148</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="T46" s="8"/>
       <c r="U46" s="8"/>
@@ -4228,13 +4233,13 @@
         <v>163</v>
       </c>
       <c r="L48" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="T48" s="1" t="s">
         <v>287</v>
       </c>
       <c r="U48" s="3" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -4242,13 +4247,13 @@
         <v>165</v>
       </c>
       <c r="N49" s="6" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="T49" s="8" t="s">
         <v>288</v>
       </c>
       <c r="U49" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="50" spans="1:21" ht="54" x14ac:dyDescent="0.15">
@@ -4305,14 +4310,21 @@
         <v>291</v>
       </c>
       <c r="R53" s="11" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+        <v>389</v>
+      </c>
+      <c r="T53" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>395</v>
+      </c>
       <c r="E54" s="5" t="s">
         <v>180</v>
       </c>
@@ -4331,20 +4343,16 @@
       <c r="P54" s="5"/>
       <c r="Q54" s="10"/>
       <c r="R54" s="10"/>
-      <c r="T54" s="1" t="s">
-        <v>292</v>
+      <c r="T54" s="8" t="s">
+        <v>293</v>
       </c>
       <c r="U54" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A55" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B55" s="5" t="s">
-        <v>175</v>
-      </c>
+      <c r="A55" s="5"/>
+      <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
@@ -4358,20 +4366,18 @@
       <c r="M55" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="N55" s="5" t="s">
-        <v>294</v>
+      <c r="N55" s="6" t="s">
+        <v>393</v>
       </c>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
       <c r="Q55" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="R55" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="T55" s="8" t="s">
-        <v>293</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="T55" s="8"/>
       <c r="U55" s="9"/>
     </row>
     <row r="56" spans="1:21" ht="54" x14ac:dyDescent="0.15">
@@ -4406,7 +4412,7 @@
         <v>200</v>
       </c>
       <c r="T57" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="U57" s="9"/>
     </row>
@@ -4425,7 +4431,7 @@
         <v>176</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5"/>
@@ -4441,7 +4447,7 @@
         <v>178</v>
       </c>
       <c r="P59" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="T59" s="8"/>
       <c r="U59" s="9"/>
@@ -4451,17 +4457,17 @@
         <v>182</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
       <c r="T60" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="U60" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.15">
@@ -4471,12 +4477,12 @@
         <v>188</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
       <c r="T61" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="U61" s="8"/>
     </row>
@@ -4494,10 +4500,10 @@
       <c r="M62" s="5"/>
       <c r="N62" s="5"/>
       <c r="Q62" s="10" t="s">
+        <v>297</v>
+      </c>
+      <c r="R62" s="10" t="s">
         <v>298</v>
-      </c>
-      <c r="R62" s="10" t="s">
-        <v>299</v>
       </c>
       <c r="T62" s="8"/>
       <c r="U62" s="8"/>
@@ -4518,10 +4524,10 @@
       <c r="Q63" s="10"/>
       <c r="R63" s="10"/>
       <c r="T63" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="U63" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
@@ -4533,7 +4539,7 @@
         <v>192</v>
       </c>
       <c r="L64" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M64" s="5"/>
       <c r="N64" s="5"/>
@@ -4546,7 +4552,7 @@
         <v>186</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
@@ -4563,19 +4569,19 @@
         <v>198</v>
       </c>
       <c r="Q66" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="R66" s="5" t="s">
         <v>302</v>
       </c>
-      <c r="R66" s="5" t="s">
-        <v>303</v>
-      </c>
       <c r="T66" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="U66" s="8"/>
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.15">
       <c r="T67" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.15">
@@ -4585,10 +4591,10 @@
     </row>
     <row r="69" spans="1:21" ht="54" x14ac:dyDescent="0.15">
       <c r="C69" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E69" s="5"/>
       <c r="F69" s="5"/>
@@ -4600,7 +4606,7 @@
         <v>206</v>
       </c>
       <c r="L69" s="5" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="70" spans="1:21" ht="54" x14ac:dyDescent="0.15">
@@ -4608,7 +4614,7 @@
         <v>208</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E70" s="5"/>
       <c r="F70" s="5"/>
@@ -4620,7 +4626,7 @@
         <v>210</v>
       </c>
       <c r="L70" s="10" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
@@ -4628,12 +4634,12 @@
         <v>212</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E71" s="5"/>
       <c r="F71" s="5"/>
       <c r="G71" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H71" s="5" t="s">
         <v>215</v>
@@ -4652,7 +4658,7 @@
         <v>216</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
@@ -4664,7 +4670,7 @@
         <v>218</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
@@ -4680,7 +4686,7 @@
         <v>220</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
@@ -4692,7 +4698,7 @@
         <v>224</v>
       </c>
       <c r="L74" s="10" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
@@ -4702,7 +4708,7 @@
         <v>222</v>
       </c>
       <c r="F75" s="6" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G75" s="5"/>
       <c r="H75" s="5"/>
@@ -4722,161 +4728,122 @@
         <v>227</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A79" s="3" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="80" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A80" s="3" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="81" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A81" s="3" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="A82" s="3" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="83" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A83" s="3" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="84" spans="1:16" ht="67.5" x14ac:dyDescent="0.15">
       <c r="G84" s="3" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="H84" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="85" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="G85" s="3" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H85" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="86" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="I86" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J86" s="3" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="87" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="I87" s="3" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J87" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="88" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="M88" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="N88" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="89" spans="1:16" ht="54" x14ac:dyDescent="0.15">
       <c r="M89" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="N89" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="90" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="O90" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="P90" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="91" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="O91" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="92" spans="1:16" ht="40.5" x14ac:dyDescent="0.15">
       <c r="O92" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="P92" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="U63:U66"/>
-    <mergeCell ref="T40:T43"/>
-    <mergeCell ref="U15:U23"/>
-    <mergeCell ref="U3:U14"/>
-    <mergeCell ref="T61:T62"/>
-    <mergeCell ref="T63:T65"/>
-    <mergeCell ref="T57:T59"/>
-    <mergeCell ref="T28:T33"/>
-    <mergeCell ref="T35:T37"/>
-    <mergeCell ref="T38:T39"/>
-    <mergeCell ref="T45:T46"/>
-    <mergeCell ref="T49:T51"/>
-    <mergeCell ref="T55:T56"/>
-    <mergeCell ref="U26:U39"/>
-    <mergeCell ref="U40:U47"/>
-    <mergeCell ref="U49:U51"/>
-    <mergeCell ref="U54:U59"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="T7:T9"/>
-    <mergeCell ref="T15:T16"/>
-    <mergeCell ref="T22:T23"/>
-    <mergeCell ref="T26:T27"/>
-    <mergeCell ref="R7:R11"/>
-    <mergeCell ref="R53:R54"/>
-    <mergeCell ref="R62:R63"/>
-    <mergeCell ref="K74:K75"/>
-    <mergeCell ref="L5:L6"/>
-    <mergeCell ref="L44:L45"/>
-    <mergeCell ref="L70:L71"/>
-    <mergeCell ref="L74:L75"/>
-    <mergeCell ref="Q7:Q11"/>
-    <mergeCell ref="K70:K71"/>
-    <mergeCell ref="Q53:Q54"/>
-    <mergeCell ref="Q62:Q63"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I37:I38"/>
     <mergeCell ref="U60:U62"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
@@ -4893,6 +4860,45 @@
     <mergeCell ref="K44:K45"/>
     <mergeCell ref="Q3:Q6"/>
     <mergeCell ref="R3:R6"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="R7:R11"/>
+    <mergeCell ref="R53:R54"/>
+    <mergeCell ref="R62:R63"/>
+    <mergeCell ref="K74:K75"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="L44:L45"/>
+    <mergeCell ref="L70:L71"/>
+    <mergeCell ref="L74:L75"/>
+    <mergeCell ref="Q7:Q11"/>
+    <mergeCell ref="K70:K71"/>
+    <mergeCell ref="Q53:Q54"/>
+    <mergeCell ref="Q62:Q63"/>
+    <mergeCell ref="U54:U59"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T7:T9"/>
+    <mergeCell ref="T15:T16"/>
+    <mergeCell ref="T22:T23"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="T54:T56"/>
+    <mergeCell ref="U63:U66"/>
+    <mergeCell ref="T40:T43"/>
+    <mergeCell ref="U15:U23"/>
+    <mergeCell ref="U3:U14"/>
+    <mergeCell ref="T61:T62"/>
+    <mergeCell ref="T63:T65"/>
+    <mergeCell ref="T57:T59"/>
+    <mergeCell ref="T28:T33"/>
+    <mergeCell ref="T35:T37"/>
+    <mergeCell ref="T38:T39"/>
+    <mergeCell ref="T45:T46"/>
+    <mergeCell ref="T49:T51"/>
+    <mergeCell ref="U26:U39"/>
+    <mergeCell ref="U40:U47"/>
+    <mergeCell ref="U49:U51"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Partially revive government policy card
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0023E225-8AFD-44D3-8E20-6E4E1571EC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE93467A-7897-4785-B315-E2E4E6FBEB23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5535" windowWidth="29475" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="原版" sheetId="1" r:id="rId1"/>
@@ -1636,7 +1636,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1646,6 +1646,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1664,7 +1670,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1698,16 +1704,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3206,11 +3218,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="C36:C37"/>
@@ -3221,11 +3233,11 @@
     <mergeCell ref="I34:I35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D74:D75"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3234,11 +3246,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U113"/>
+  <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P97" sqref="P97"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25:L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3353,10 +3365,10 @@
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-      <c r="Q3" s="11" t="s">
+      <c r="Q3" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="R3" s="12" t="s">
+      <c r="R3" s="11" t="s">
         <v>369</v>
       </c>
       <c r="T3" s="10" t="s">
@@ -3387,8 +3399,8 @@
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
       <c r="T4" s="9"/>
       <c r="U4" s="10"/>
     </row>
@@ -3403,18 +3415,18 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
-      <c r="K5" s="6" t="s">
+      <c r="K5" s="15" t="s">
         <v>418</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="L5" s="15" t="s">
         <v>420</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
       <c r="U5" s="10"/>
     </row>
     <row r="6" spans="1:21" ht="27" x14ac:dyDescent="0.15">
@@ -3432,18 +3444,18 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="11" t="s">
+      <c r="K6" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="L6" s="12" t="s">
+      <c r="L6" s="14" t="s">
         <v>332</v>
       </c>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
       <c r="T6" s="1" t="s">
         <v>256</v>
       </c>
@@ -3464,14 +3476,14 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
       <c r="T7" s="1" t="s">
         <v>257</v>
       </c>
@@ -3510,10 +3522,10 @@
       </c>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-      <c r="Q8" s="11" t="s">
+      <c r="Q8" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="R8" s="11" t="s">
+      <c r="R8" s="12" t="s">
         <v>259</v>
       </c>
       <c r="T8" s="9" t="s">
@@ -3550,8 +3562,8 @@
       </c>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
       <c r="T9" s="9"/>
       <c r="U9" s="10"/>
     </row>
@@ -3584,8 +3596,8 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
       <c r="T10" s="9"/>
       <c r="U10" s="10"/>
     </row>
@@ -3614,8 +3626,8 @@
       <c r="P11" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
       <c r="T11" s="1" t="s">
         <v>261</v>
       </c>
@@ -3642,8 +3654,8 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
+      <c r="Q12" s="12"/>
+      <c r="R12" s="12"/>
       <c r="T12" s="1" t="s">
         <v>262</v>
       </c>
@@ -3754,7 +3766,7 @@
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="12" t="s">
         <v>63</v>
       </c>
       <c r="J16" s="7" t="s">
@@ -3792,7 +3804,7 @@
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
-      <c r="I17" s="11"/>
+      <c r="I17" s="12"/>
       <c r="J17" s="6" t="s">
         <v>309</v>
       </c>
@@ -3818,10 +3830,10 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="15" t="s">
         <v>415</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="L18" s="15" t="s">
         <v>416</v>
       </c>
       <c r="M18" s="5"/>
@@ -3921,10 +3933,10 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
-      <c r="K21" s="6" t="s">
+      <c r="K21" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="L21" s="6" t="s">
+      <c r="L21" s="15" t="s">
         <v>355</v>
       </c>
       <c r="M21" s="5"/>
@@ -4041,10 +4053,10 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="16" t="s">
         <v>270</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="15" t="s">
         <v>328</v>
       </c>
       <c r="M25" s="5"/>
@@ -4061,46 +4073,20 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A28" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.15">
       <c r="E28" s="5" t="s">
         <v>91</v>
       </c>
       <c r="F28" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
-      <c r="P28" s="5"/>
-      <c r="Q28" s="5"/>
-      <c r="R28" s="5"/>
-      <c r="T28" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="U28" s="10" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    </row>
+    <row r="29" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -4110,10 +4096,10 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="6" t="s">
+      <c r="K29" s="14" t="s">
         <v>375</v>
       </c>
-      <c r="L29" s="7" t="s">
+      <c r="L29" s="14" t="s">
         <v>407</v>
       </c>
       <c r="M29" s="5"/>
@@ -4122,52 +4108,50 @@
       <c r="P29" s="5"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="5"/>
-      <c r="S29" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="T29" s="9"/>
-      <c r="U29" s="10"/>
-    </row>
-    <row r="30" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>130</v>
-      </c>
+      <c r="T29" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="U29" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="A30" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="L30" s="5" t="s">
-        <v>132</v>
-      </c>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
       <c r="P30" s="5"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="5"/>
-      <c r="T30" s="10" t="s">
-        <v>306</v>
-      </c>
+      <c r="S30" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="T30" s="9"/>
       <c r="U30" s="10"/>
     </row>
     <row r="31" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A31" s="5"/>
       <c r="B31" s="5"/>
       <c r="C31" s="5" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -4175,11 +4159,11 @@
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="11" t="s">
-        <v>135</v>
+      <c r="K31" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="L31" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M31" s="5"/>
       <c r="N31" s="5"/>
@@ -4187,27 +4171,31 @@
       <c r="P31" s="5"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="5"/>
-      <c r="T31" s="9"/>
+      <c r="T31" s="10" t="s">
+        <v>306</v>
+      </c>
       <c r="U31" s="10"/>
     </row>
     <row r="32" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>137</v>
-      </c>
+      <c r="C32" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
       <c r="G32" s="5"/>
       <c r="H32" s="5"/>
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="11"/>
+      <c r="K32" s="12" t="s">
+        <v>135</v>
+      </c>
       <c r="L32" s="5" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="M32" s="5"/>
       <c r="N32" s="5"/>
@@ -4218,29 +4206,27 @@
       <c r="T32" s="9"/>
       <c r="U32" s="10"/>
     </row>
-    <row r="33" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>376</v>
-      </c>
+      <c r="K33" s="12"/>
+      <c r="L33" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
       <c r="O33" s="5"/>
       <c r="P33" s="5"/>
       <c r="Q33" s="5"/>
@@ -4253,492 +4239,492 @@
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
-      <c r="I34" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>360</v>
-      </c>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>376</v>
+      </c>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
       <c r="T34" s="9"/>
       <c r="U34" s="10"/>
     </row>
-    <row r="35" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
-      <c r="A35" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>99</v>
-      </c>
+    <row r="35" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
-      <c r="E35" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" s="5" t="s">
-        <v>274</v>
-      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="5"/>
       <c r="H35" s="5"/>
       <c r="I35" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>275</v>
+        <v>157</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>360</v>
       </c>
       <c r="T35" s="9"/>
       <c r="U35" s="10"/>
     </row>
-    <row r="36" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="P36" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>276</v>
-      </c>
+      <c r="E36" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="T36" s="9"/>
       <c r="U36" s="10"/>
     </row>
     <row r="37" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="A37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>105</v>
+      </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
+      <c r="G37" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
-      <c r="K37" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>160</v>
-      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
       <c r="M37" s="5"/>
       <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
-      <c r="P37" s="5"/>
-      <c r="T37" s="9" t="s">
-        <v>277</v>
+      <c r="O37" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="P37" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="T37" s="1" t="s">
+        <v>276</v>
       </c>
       <c r="U37" s="10"/>
     </row>
-    <row r="38" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="A38" s="5"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
-      <c r="E38" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>139</v>
-      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
-      <c r="I38" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="J38" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+      <c r="K38" s="16" t="s">
+        <v>278</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>160</v>
+      </c>
       <c r="M38" s="5"/>
       <c r="N38" s="5"/>
       <c r="O38" s="5"/>
       <c r="P38" s="5"/>
-      <c r="T38" s="9"/>
+      <c r="T38" s="9" t="s">
+        <v>277</v>
+      </c>
       <c r="U38" s="10"/>
     </row>
-    <row r="39" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="C39" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>421</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
+    <row r="39" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>139</v>
+      </c>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
-      <c r="I39" s="11" t="s">
-        <v>118</v>
+      <c r="I39" s="5" t="s">
+        <v>140</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>421</v>
-      </c>
+        <v>326</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+      <c r="P39" s="5"/>
       <c r="T39" s="9"/>
       <c r="U39" s="10"/>
     </row>
     <row r="40" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="C40" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>421</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="5" t="s">
+      <c r="I40" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>421</v>
+      </c>
+      <c r="T40" s="9"/>
+      <c r="U40" s="10"/>
+    </row>
+    <row r="41" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="C41" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="T40" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="U40" s="10"/>
-    </row>
-    <row r="41" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
-      <c r="T41" s="9"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="12"/>
+      <c r="J41" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="T41" s="9" t="s">
+        <v>280</v>
+      </c>
       <c r="U41" s="10"/>
     </row>
-    <row r="42" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5" t="s">
-        <v>152</v>
+        <v>95</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
-      <c r="T42" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="U42" s="10" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="T42" s="9"/>
+      <c r="U42" s="10"/>
+    </row>
+    <row r="43" spans="1:21" ht="54" x14ac:dyDescent="0.15">
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="S43" s="4"/>
-      <c r="T43" s="9"/>
-      <c r="U43" s="9"/>
+      <c r="G43" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>366</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5"/>
+      <c r="T43" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="U43" s="10" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="44" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="E44" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>368</v>
-      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
-      <c r="S44" s="2"/>
+      <c r="I44" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="J44" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="S44" s="4"/>
       <c r="T44" s="9"/>
       <c r="U44" s="9"/>
     </row>
-    <row r="45" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A45" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+    <row r="45" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="E45" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>113</v>
+        <v>148</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>368</v>
       </c>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
-      <c r="I45" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="J45" s="5" t="s">
-        <v>115</v>
-      </c>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="S45" s="2"/>
       <c r="T45" s="9"/>
       <c r="U45" s="9"/>
     </row>
     <row r="46" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="C46" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>122</v>
-      </c>
+      <c r="A46" s="6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>354</v>
+        <v>112</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>113</v>
       </c>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
-      <c r="K46" s="11" t="s">
+      <c r="I46" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="T46" s="9"/>
+      <c r="U46" s="9"/>
+    </row>
+    <row r="47" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="C47" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="D47" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5"/>
+      <c r="K47" s="13" t="s">
         <v>281</v>
       </c>
-      <c r="L46" s="12" t="s">
+      <c r="L47" s="14" t="s">
         <v>362</v>
       </c>
-      <c r="T46" s="1" t="s">
+      <c r="T47" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="U46" s="9"/>
-    </row>
-    <row r="47" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5" t="s">
+      <c r="U47" s="9"/>
+    </row>
+    <row r="48" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="H47" s="6" t="s">
+      <c r="H48" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="T47" s="9" t="s">
+      <c r="K48" s="13"/>
+      <c r="L48" s="13"/>
+      <c r="T48" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="U47" s="9"/>
-    </row>
-    <row r="48" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="E48" s="5" t="s">
+      <c r="U48" s="9"/>
+    </row>
+    <row r="49" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="E49" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F48" s="6" t="s">
+      <c r="F49" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="T48" s="9"/>
-      <c r="U48" s="9"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="E49" s="5" t="s">
+      <c r="T49" s="9"/>
+      <c r="U49" s="9"/>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="E50" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F50" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="5"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="T49" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="U49" s="9"/>
-    </row>
-    <row r="50" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
-      <c r="K50" s="5" t="s">
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="T50" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="U50" s="9"/>
+    </row>
+    <row r="51" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="L50" s="6" t="s">
+      <c r="L51" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="T50" s="1" t="s">
+      <c r="T51" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="U50" s="3" t="s">
+      <c r="U51" s="3" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="51" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M51" s="5" t="s">
+    <row r="52" spans="1:21" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M52" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="N51" s="6" t="s">
+      <c r="N52" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="T51" s="9" t="s">
+      <c r="T52" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="U51" s="10" t="s">
+      <c r="U52" s="10" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="52" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="M52" s="5" t="s">
+    <row r="53" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="M53" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="N52" s="5" t="s">
+      <c r="N53" s="5" t="s">
         <v>166</v>
       </c>
-      <c r="Q52" s="5" t="s">
+      <c r="Q53" s="5" t="s">
         <v>286</v>
       </c>
-      <c r="R52" s="5" t="s">
+      <c r="R53" s="5" t="s">
         <v>287</v>
       </c>
-      <c r="T52" s="9"/>
-      <c r="U52" s="9"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.15">
       <c r="T53" s="9"/>
       <c r="U53" s="9"/>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A54" s="1" t="s">
+      <c r="T54" s="9"/>
+      <c r="U54" s="9"/>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A55" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="55" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A55" s="5" t="s">
+    <row r="56" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="A56" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B56" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
-      <c r="K55" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
-      <c r="P55" s="5"/>
-      <c r="Q55" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="R55" s="12" t="s">
-        <v>377</v>
-      </c>
-      <c r="T55" s="1" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A56" s="5"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="D56" s="6" t="s">
-        <v>404</v>
-      </c>
-      <c r="E56" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="F56" s="5" t="s">
-        <v>179</v>
-      </c>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
       <c r="G56" s="5"/>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
       <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
+      <c r="K56" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>171</v>
+      </c>
       <c r="M56" s="5"/>
       <c r="N56" s="5"/>
       <c r="O56" s="5"/>
       <c r="P56" s="5"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="11"/>
-      <c r="T56" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="U56" s="10" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
+      <c r="Q56" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="R56" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="T56" s="1" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.15">
       <c r="A57" s="5"/>
       <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
+      <c r="C57" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>179</v>
+      </c>
       <c r="G57" s="5"/>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
       <c r="J57" s="5"/>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
-      <c r="M57" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="N57" s="6" t="s">
-        <v>381</v>
-      </c>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
       <c r="O57" s="5"/>
       <c r="P57" s="5"/>
-      <c r="Q57" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="R57" s="6" t="s">
-        <v>382</v>
-      </c>
-      <c r="T57" s="9"/>
-      <c r="U57" s="10"/>
-    </row>
-    <row r="58" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="Q57" s="12"/>
+      <c r="R57" s="12"/>
+      <c r="T57" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="U57" s="10" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" ht="67.5" x14ac:dyDescent="0.15">
       <c r="A58" s="5"/>
       <c r="B58" s="5"/>
       <c r="C58" s="5"/>
@@ -4747,235 +4733,243 @@
       <c r="F58" s="5"/>
       <c r="G58" s="5"/>
       <c r="H58" s="5"/>
-      <c r="I58" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>189</v>
-      </c>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
+      <c r="M58" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="N58" s="6" t="s">
+        <v>381</v>
+      </c>
       <c r="O58" s="5"/>
       <c r="P58" s="5"/>
+      <c r="Q58" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="R58" s="6" t="s">
+        <v>382</v>
+      </c>
       <c r="T58" s="9"/>
       <c r="U58" s="10"/>
     </row>
-    <row r="59" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="O59" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="P59" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="T59" s="10" t="s">
-        <v>323</v>
-      </c>
+    <row r="59" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="A59" s="5"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="5"/>
+      <c r="F59" s="5"/>
+      <c r="G59" s="5"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
+      <c r="P59" s="5"/>
+      <c r="T59" s="9"/>
       <c r="U59" s="10"/>
     </row>
     <row r="60" spans="1:21" ht="27" x14ac:dyDescent="0.15">
       <c r="O60" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="P60" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="T60" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="U60" s="10"/>
+    </row>
+    <row r="61" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="O61" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="P60" s="5" t="s">
+      <c r="P61" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="T60" s="10"/>
-      <c r="U60" s="10"/>
-    </row>
-    <row r="61" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="C61" s="5" t="s">
+      <c r="T61" s="10"/>
+      <c r="U61" s="10"/>
+    </row>
+    <row r="62" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="C62" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D62" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="P61" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="T61" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="U61" s="10"/>
-    </row>
-    <row r="62" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="G62" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="H62" s="6" t="s">
-        <v>357</v>
-      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
       <c r="I62" s="5"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
-      <c r="T62" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="U62" s="10" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="J63" s="6" t="s">
-        <v>370</v>
-      </c>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="P62" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="T62" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="U62" s="10"/>
+    </row>
+    <row r="63" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="G63" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="H63" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
-      <c r="T63" s="9"/>
-      <c r="U63" s="9"/>
-    </row>
-    <row r="64" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G64" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
+      <c r="T63" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="U63" s="10" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="27" x14ac:dyDescent="0.15">
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>370</v>
+      </c>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="Q64" s="11" t="s">
-        <v>294</v>
-      </c>
-      <c r="R64" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="T64" s="9" t="s">
-        <v>296</v>
-      </c>
+      <c r="T64" s="9"/>
       <c r="U64" s="9"/>
     </row>
-    <row r="65" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
+    <row r="65" spans="1:21" ht="55.9" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G65" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>183</v>
+      </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
-      <c r="M65" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="N65" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="Q65" s="11"/>
-      <c r="R65" s="11"/>
-      <c r="T65" s="9"/>
-      <c r="U65" s="10" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="66" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="Q65" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="R65" s="12" t="s">
+        <v>295</v>
+      </c>
+      <c r="T65" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="U65" s="9"/>
+    </row>
+    <row r="66" spans="1:21" ht="54" x14ac:dyDescent="0.15">
       <c r="G66" s="5"/>
       <c r="H66" s="5"/>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
-      <c r="K66" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="L66" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="M66" s="5"/>
-      <c r="N66" s="5"/>
-      <c r="P66" s="2"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="N66" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q66" s="12"/>
+      <c r="R66" s="12"/>
       <c r="T66" s="9"/>
-      <c r="U66" s="9"/>
-    </row>
-    <row r="67" spans="1:21" ht="81" x14ac:dyDescent="0.15">
-      <c r="G67" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>310</v>
-      </c>
+      <c r="U66" s="10" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="G67" s="5"/>
+      <c r="H67" s="5"/>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
-      <c r="K67" s="5"/>
-      <c r="L67" s="5"/>
-      <c r="M67" s="6" t="s">
+      <c r="K67" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="L67" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="M67" s="5"/>
+      <c r="N67" s="5"/>
+      <c r="P67" s="2"/>
+      <c r="T67" s="9"/>
+      <c r="U67" s="9"/>
+    </row>
+    <row r="68" spans="1:21" ht="81" x14ac:dyDescent="0.15">
+      <c r="G68" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="I68" s="5"/>
+      <c r="J68" s="5"/>
+      <c r="K68" s="15" t="s">
         <v>412</v>
       </c>
-      <c r="N67" s="6" t="s">
+      <c r="L68" s="15" t="s">
         <v>413</v>
       </c>
-      <c r="T67" s="2" t="s">
+      <c r="T68" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="U67" s="9"/>
-    </row>
-    <row r="68" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="O68" s="5" t="s">
+      <c r="U68" s="9"/>
+    </row>
+    <row r="69" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="O69" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="P68" s="5" t="s">
+      <c r="P69" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="Q68" s="5" t="s">
+      <c r="Q69" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="R68" s="5" t="s">
+      <c r="R69" s="5" t="s">
         <v>299</v>
       </c>
-      <c r="T68" s="1" t="s">
+      <c r="T69" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="U68" s="9"/>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A70" s="1" t="s">
+      <c r="U69" s="9"/>
+    </row>
+    <row r="71" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A71" s="1" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="71" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="C71" s="6" t="s">
+    <row r="72" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C72" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="D71" s="6" t="s">
+      <c r="D72" s="6" t="s">
         <v>315</v>
-      </c>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
-      <c r="J71" s="5"/>
-      <c r="K71" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="L71" s="5" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="72" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="C72" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>316</v>
       </c>
       <c r="E72" s="5"/>
       <c r="F72" s="5"/>
@@ -4983,60 +4977,64 @@
       <c r="H72" s="5"/>
       <c r="I72" s="5"/>
       <c r="J72" s="5"/>
-      <c r="K72" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="L72" s="11" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="73" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C73" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D73" s="12" t="s">
-        <v>314</v>
+      <c r="K72" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="L72" s="5" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="73" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C73" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="E73" s="5"/>
       <c r="F73" s="5"/>
-      <c r="G73" s="6" t="s">
-        <v>379</v>
-      </c>
-      <c r="H73" s="5" t="s">
-        <v>213</v>
-      </c>
+      <c r="G73" s="5"/>
+      <c r="H73" s="5"/>
       <c r="I73" s="5"/>
       <c r="J73" s="5"/>
-      <c r="K73" s="11"/>
-      <c r="L73" s="11"/>
-    </row>
-    <row r="74" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="C74" s="11"/>
-      <c r="D74" s="11"/>
+      <c r="K73" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="L73" s="12" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="74" spans="1:21" ht="74.099999999999994" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C74" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>314</v>
+      </c>
       <c r="E74" s="5"/>
       <c r="F74" s="5"/>
-      <c r="G74" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H74" s="6" t="s">
-        <v>378</v>
+      <c r="G74" s="6" t="s">
+        <v>379</v>
+      </c>
+      <c r="H74" s="5" t="s">
+        <v>213</v>
       </c>
       <c r="I74" s="5"/>
       <c r="J74" s="5"/>
-      <c r="K74" s="5"/>
-      <c r="L74" s="5"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
     </row>
     <row r="75" spans="1:21" ht="54" x14ac:dyDescent="0.15">
-      <c r="C75" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>303</v>
-      </c>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
       <c r="E75" s="5"/>
       <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
+      <c r="G75" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="H75" s="6" t="s">
+        <v>378</v>
+      </c>
       <c r="I75" s="5"/>
       <c r="J75" s="5"/>
       <c r="K75" s="5"/>
@@ -5044,10 +5042,10 @@
     </row>
     <row r="76" spans="1:21" ht="54" x14ac:dyDescent="0.15">
       <c r="C76" s="5" t="s">
-        <v>218</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>317</v>
+        <v>216</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>303</v>
       </c>
       <c r="E76" s="5"/>
       <c r="F76" s="5"/>
@@ -5055,259 +5053,261 @@
       <c r="H76" s="5"/>
       <c r="I76" s="5"/>
       <c r="J76" s="5"/>
-      <c r="K76" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="L76" s="11" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="77" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="F77" s="6" t="s">
-        <v>318</v>
-      </c>
+      <c r="K76" s="5"/>
+      <c r="L76" s="5"/>
+    </row>
+    <row r="77" spans="1:21" ht="54" x14ac:dyDescent="0.15">
+      <c r="C77" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5"/>
       <c r="G77" s="5"/>
       <c r="H77" s="5"/>
       <c r="I77" s="5"/>
       <c r="J77" s="5"/>
-      <c r="K77" s="11"/>
-      <c r="L77" s="11"/>
+      <c r="K77" s="12" t="s">
+        <v>222</v>
+      </c>
+      <c r="L77" s="12" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="78" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
+      <c r="E78" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>318</v>
+      </c>
       <c r="G78" s="5"/>
       <c r="H78" s="5"/>
-      <c r="I78" s="5" t="s">
+      <c r="I78" s="5"/>
+      <c r="J78" s="5"/>
+      <c r="K78" s="12"/>
+      <c r="L78" s="12"/>
+    </row>
+    <row r="79" spans="1:21" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="C79" s="5"/>
+      <c r="D79" s="5"/>
+      <c r="E79" s="5"/>
+      <c r="F79" s="5"/>
+      <c r="G79" s="5"/>
+      <c r="H79" s="5"/>
+      <c r="I79" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="J78" s="6" t="s">
+      <c r="J79" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="K78" s="5"/>
-      <c r="L78" s="5"/>
-    </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A81" s="3" t="s">
+      <c r="K79" s="5"/>
+      <c r="L79" s="5"/>
+    </row>
+    <row r="82" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A82" s="3" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="82" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="B82" s="12" t="s">
-        <v>401</v>
-      </c>
-      <c r="C82" s="12"/>
-      <c r="D82" s="12"/>
-      <c r="E82" s="12"/>
-      <c r="F82" s="12"/>
     </row>
     <row r="83" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A83" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="B83" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11"/>
+      <c r="E83" s="11"/>
+      <c r="F83" s="11"/>
+    </row>
+    <row r="84" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="B83" s="12" t="s">
+      <c r="B84" s="11" t="s">
         <v>423</v>
       </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12"/>
-      <c r="E83" s="12"/>
-      <c r="F83" s="12"/>
-      <c r="G83" s="12"/>
-      <c r="H83" s="12"/>
-    </row>
-    <row r="84" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="6" t="s">
+      <c r="C84" s="11"/>
+      <c r="D84" s="11"/>
+      <c r="E84" s="11"/>
+      <c r="F84" s="11"/>
+      <c r="G84" s="11"/>
+      <c r="H84" s="11"/>
+    </row>
+    <row r="85" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B85" s="11" t="s">
         <v>402</v>
       </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12"/>
-      <c r="E84" s="12"/>
-      <c r="F84" s="12"/>
-      <c r="G84" s="12"/>
-      <c r="H84" s="12"/>
-    </row>
-    <row r="85" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="6" t="s">
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+      <c r="E85" s="11"/>
+      <c r="F85" s="11"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="11"/>
+    </row>
+    <row r="86" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="B85" s="12" t="s">
+      <c r="B86" s="11" t="s">
         <v>399</v>
       </c>
-      <c r="C85" s="12"/>
-      <c r="D85" s="12"/>
-      <c r="E85" s="12"/>
-      <c r="F85" s="12"/>
-      <c r="G85" s="12"/>
-      <c r="H85" s="12"/>
-      <c r="I85" s="12"/>
-      <c r="J85" s="12"/>
-    </row>
-    <row r="86" spans="1:18" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G86" s="6" t="s">
+      <c r="C86" s="11"/>
+      <c r="D86" s="11"/>
+      <c r="E86" s="11"/>
+      <c r="F86" s="11"/>
+      <c r="G86" s="11"/>
+      <c r="H86" s="11"/>
+      <c r="I86" s="11"/>
+      <c r="J86" s="11"/>
+    </row>
+    <row r="87" spans="1:18" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G87" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="H86" s="12" t="s">
+      <c r="H87" s="11" t="s">
         <v>422</v>
       </c>
-      <c r="I86" s="12"/>
-      <c r="J86" s="12"/>
-      <c r="K86" s="12"/>
-      <c r="L86" s="12"/>
-    </row>
-    <row r="87" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G87" s="6" t="s">
+      <c r="I87" s="11"/>
+      <c r="J87" s="11"/>
+      <c r="K87" s="11"/>
+      <c r="L87" s="11"/>
+    </row>
+    <row r="88" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G88" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="H87" s="12" t="s">
+      <c r="H88" s="11" t="s">
         <v>400</v>
       </c>
-      <c r="I87" s="12"/>
-      <c r="J87" s="12"/>
-      <c r="K87" s="12"/>
-      <c r="L87" s="12"/>
-      <c r="M87" s="12"/>
-      <c r="N87" s="12"/>
-    </row>
-    <row r="88" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I88" s="3" t="s">
+      <c r="I88" s="11"/>
+      <c r="J88" s="11"/>
+      <c r="K88" s="11"/>
+      <c r="L88" s="11"/>
+      <c r="M88" s="11"/>
+      <c r="N88" s="11"/>
+    </row>
+    <row r="89" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I89" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="J88" s="10" t="s">
+      <c r="J89" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="K88" s="10"/>
-      <c r="L88" s="10"/>
-      <c r="M88" s="10"/>
-      <c r="N88" s="10"/>
-      <c r="O88" s="10"/>
-      <c r="P88" s="10"/>
-      <c r="Q88" s="10"/>
-      <c r="R88" s="10"/>
-    </row>
-    <row r="89" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I89" s="6" t="s">
+      <c r="K89" s="10"/>
+      <c r="L89" s="10"/>
+      <c r="M89" s="10"/>
+      <c r="N89" s="10"/>
+      <c r="O89" s="10"/>
+      <c r="P89" s="10"/>
+      <c r="Q89" s="10"/>
+      <c r="R89" s="10"/>
+    </row>
+    <row r="90" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I90" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="J89" s="12" t="s">
+      <c r="J90" s="11" t="s">
         <v>425</v>
       </c>
-      <c r="K89" s="12"/>
-      <c r="L89" s="12"/>
-      <c r="M89" s="12"/>
-      <c r="N89" s="12"/>
-    </row>
-    <row r="90" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M90" s="13" t="s">
+      <c r="K90" s="11"/>
+      <c r="L90" s="11"/>
+      <c r="M90" s="11"/>
+      <c r="N90" s="11"/>
+    </row>
+    <row r="91" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M91" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="N90" s="14" t="s">
+      <c r="N91" s="10" t="s">
         <v>403</v>
-      </c>
-      <c r="O90" s="14"/>
-      <c r="P90" s="14"/>
-      <c r="Q90" s="14"/>
-      <c r="R90" s="14"/>
-    </row>
-    <row r="91" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M91" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="N91" s="10" t="s">
-        <v>345</v>
       </c>
       <c r="O91" s="10"/>
       <c r="P91" s="10"/>
       <c r="Q91" s="10"/>
       <c r="R91" s="10"/>
     </row>
-    <row r="92" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O92" s="6" t="s">
+    <row r="92" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M92" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="N92" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="O92" s="10"/>
+      <c r="P92" s="10"/>
+      <c r="Q92" s="10"/>
+      <c r="R92" s="10"/>
+    </row>
+    <row r="93" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O93" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="P92" s="12" t="s">
+      <c r="P93" s="11" t="s">
         <v>347</v>
       </c>
-      <c r="Q92" s="12"/>
-      <c r="R92" s="12"/>
-    </row>
-    <row r="93" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O93" s="3" t="s">
-        <v>348</v>
-      </c>
-      <c r="P93" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="Q93" s="10"/>
-      <c r="R93" s="10"/>
+      <c r="Q93" s="11"/>
+      <c r="R93" s="11"/>
     </row>
     <row r="94" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O94" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="P94" s="10" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="Q94" s="10"/>
       <c r="R94" s="10"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A96" s="3" t="s">
+    <row r="95" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="O95" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="P95" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="Q95" s="10"/>
+      <c r="R95" s="10"/>
+    </row>
+    <row r="97" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A97" s="3" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="97" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="3" t="s">
+    <row r="98" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="3" t="s">
         <v>334</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B98" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="C97" s="10"/>
-      <c r="D97" s="10"/>
-      <c r="E97" s="10"/>
-      <c r="F97" s="10"/>
-    </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A98" s="3" t="s">
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="F98" s="10"/>
+    </row>
+    <row r="99" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A99" s="3" t="s">
         <v>335</v>
       </c>
-      <c r="B98" s="8" t="s">
+      <c r="B99" s="8" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="99" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="3" t="s">
+    <row r="100" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="B99" s="10" t="s">
+      <c r="B100" s="10" t="s">
         <v>386</v>
-      </c>
-      <c r="C99" s="10"/>
-      <c r="D99" s="10"/>
-      <c r="E99" s="10"/>
-      <c r="F99" s="10"/>
-      <c r="G99" s="10"/>
-      <c r="H99" s="10"/>
-    </row>
-    <row r="100" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="3" t="s">
-        <v>337</v>
-      </c>
-      <c r="B100" s="10" t="s">
-        <v>387</v>
       </c>
       <c r="C100" s="10"/>
       <c r="D100" s="10"/>
@@ -5317,14 +5317,14 @@
       <c r="H100" s="10"/>
     </row>
     <row r="101" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="3"/>
-      <c r="B101" s="3"/>
-      <c r="C101" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>392</v>
-      </c>
+      <c r="A101" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B101" s="10" t="s">
+        <v>387</v>
+      </c>
+      <c r="C101" s="10"/>
+      <c r="D101" s="10"/>
       <c r="E101" s="10"/>
       <c r="F101" s="10"/>
       <c r="G101" s="10"/>
@@ -5333,219 +5333,168 @@
     <row r="102" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A102" s="3"/>
       <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3" t="s">
+      <c r="C102" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="D102" s="10" t="s">
+        <v>392</v>
+      </c>
+      <c r="E102" s="10"/>
+      <c r="F102" s="10"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="10"/>
+    </row>
+    <row r="103" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="3"/>
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
+      <c r="E103" s="3"/>
+      <c r="F103" s="3"/>
+      <c r="G103" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="H102" s="10" t="s">
+      <c r="H103" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="I102" s="10"/>
-      <c r="J102" s="10"/>
-      <c r="K102" s="10"/>
-      <c r="L102" s="10"/>
-    </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="G103" s="3" t="s">
+      <c r="I103" s="10"/>
+      <c r="J103" s="10"/>
+      <c r="K103" s="10"/>
+      <c r="L103" s="10"/>
+    </row>
+    <row r="104" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="G104" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="H103" s="8" t="s">
+      <c r="H104" s="8" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="104" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="G104" s="3" t="s">
+    <row r="105" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="G105" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="H104" s="10" t="s">
+      <c r="H105" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="I104" s="10"/>
-      <c r="J104" s="10"/>
-      <c r="K104" s="10"/>
-      <c r="L104" s="10"/>
-      <c r="M104" s="10"/>
-      <c r="N104" s="10"/>
-    </row>
-    <row r="105" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I105" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="J105" s="10" t="s">
-        <v>389</v>
-      </c>
+      <c r="I105" s="10"/>
+      <c r="J105" s="10"/>
       <c r="K105" s="10"/>
       <c r="L105" s="10"/>
       <c r="M105" s="10"/>
       <c r="N105" s="10"/>
-      <c r="O105" s="10"/>
-      <c r="P105" s="10"/>
-      <c r="Q105" s="10"/>
-      <c r="R105" s="10"/>
-    </row>
-    <row r="106" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+    </row>
+    <row r="106" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I106" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="J106" s="10" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K106" s="10"/>
       <c r="L106" s="10"/>
       <c r="M106" s="10"/>
       <c r="N106" s="10"/>
+      <c r="O106" s="10"/>
+      <c r="P106" s="10"/>
+      <c r="Q106" s="10"/>
+      <c r="R106" s="10"/>
     </row>
     <row r="107" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I107" s="3" t="s">
-        <v>394</v>
+        <v>341</v>
       </c>
       <c r="J107" s="10" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="K107" s="10"/>
       <c r="L107" s="10"/>
-      <c r="M107" s="3"/>
-      <c r="N107" s="3"/>
+      <c r="M107" s="10"/>
+      <c r="N107" s="10"/>
     </row>
     <row r="108" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I108" s="3" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="J108" s="10" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="K108" s="10"/>
       <c r="L108" s="10"/>
-      <c r="M108" s="10"/>
-      <c r="N108" s="10"/>
-    </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="M109" s="3" t="s">
+      <c r="M108" s="3"/>
+      <c r="N108" s="3"/>
+    </row>
+    <row r="109" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="I109" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="J109" s="10" t="s">
+        <v>398</v>
+      </c>
+      <c r="K109" s="10"/>
+      <c r="L109" s="10"/>
+      <c r="M109" s="10"/>
+      <c r="N109" s="10"/>
+    </row>
+    <row r="110" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="M110" s="3" t="s">
         <v>342</v>
       </c>
-      <c r="N109" s="10" t="s">
+      <c r="N110" s="10" t="s">
         <v>343</v>
-      </c>
-      <c r="O109" s="10"/>
-      <c r="P109" s="10"/>
-      <c r="Q109" s="10"/>
-      <c r="R109" s="10"/>
-    </row>
-    <row r="110" spans="1:18" ht="27" x14ac:dyDescent="0.15">
-      <c r="M110" s="3" t="s">
-        <v>344</v>
-      </c>
-      <c r="N110" s="10" t="s">
-        <v>345</v>
       </c>
       <c r="O110" s="10"/>
       <c r="P110" s="10"/>
       <c r="Q110" s="10"/>
       <c r="R110" s="10"/>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="O111" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="P111" s="10" t="s">
-        <v>347</v>
-      </c>
+    <row r="111" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+      <c r="M111" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="N111" s="10" t="s">
+        <v>345</v>
+      </c>
+      <c r="O111" s="10"/>
+      <c r="P111" s="10"/>
       <c r="Q111" s="10"/>
       <c r="R111" s="10"/>
     </row>
-    <row r="112" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.15">
       <c r="O112" s="3" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="P112" s="10" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="Q112" s="10"/>
       <c r="R112" s="10"/>
     </row>
-    <row r="113" spans="15:18" x14ac:dyDescent="0.15">
+    <row r="113" spans="15:18" ht="27" x14ac:dyDescent="0.15">
       <c r="O113" s="3" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="P113" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="Q113" s="10"/>
       <c r="R113" s="10"/>
     </row>
+    <row r="114" spans="15:18" x14ac:dyDescent="0.15">
+      <c r="O114" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="P114" s="10" t="s">
+        <v>351</v>
+      </c>
+      <c r="Q114" s="10"/>
+      <c r="R114" s="10"/>
+    </row>
   </sheetData>
-  <mergeCells count="83">
-    <mergeCell ref="P113:R113"/>
-    <mergeCell ref="J106:N106"/>
-    <mergeCell ref="J105:R105"/>
-    <mergeCell ref="H104:N104"/>
-    <mergeCell ref="H102:L102"/>
-    <mergeCell ref="J107:L107"/>
-    <mergeCell ref="J108:N108"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="N109:R109"/>
-    <mergeCell ref="N110:R110"/>
-    <mergeCell ref="P111:R111"/>
-    <mergeCell ref="P112:R112"/>
-    <mergeCell ref="D101:H101"/>
-    <mergeCell ref="P92:R92"/>
-    <mergeCell ref="P93:R93"/>
-    <mergeCell ref="P94:R94"/>
-    <mergeCell ref="B97:F97"/>
-    <mergeCell ref="B99:H99"/>
-    <mergeCell ref="H87:N87"/>
-    <mergeCell ref="J88:R88"/>
-    <mergeCell ref="J89:N89"/>
-    <mergeCell ref="N90:R90"/>
-    <mergeCell ref="N91:R91"/>
-    <mergeCell ref="B82:F82"/>
-    <mergeCell ref="B83:H83"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B85:J85"/>
-    <mergeCell ref="H86:L86"/>
-    <mergeCell ref="U65:U68"/>
-    <mergeCell ref="T42:T45"/>
-    <mergeCell ref="U16:U25"/>
-    <mergeCell ref="U3:U15"/>
-    <mergeCell ref="T30:T35"/>
-    <mergeCell ref="T37:T39"/>
-    <mergeCell ref="T40:T41"/>
-    <mergeCell ref="T47:T48"/>
-    <mergeCell ref="T51:T53"/>
-    <mergeCell ref="U28:U41"/>
-    <mergeCell ref="U42:U49"/>
-    <mergeCell ref="U51:U53"/>
-    <mergeCell ref="U56:U61"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="T8:T10"/>
-    <mergeCell ref="T16:T17"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="T28:T29"/>
-    <mergeCell ref="T56:T58"/>
-    <mergeCell ref="R8:R12"/>
-    <mergeCell ref="R55:R56"/>
-    <mergeCell ref="R64:R65"/>
-    <mergeCell ref="K76:K77"/>
-    <mergeCell ref="K72:K73"/>
-    <mergeCell ref="T59:T60"/>
-    <mergeCell ref="T64:T66"/>
-    <mergeCell ref="T62:T63"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="L46:L47"/>
-    <mergeCell ref="L72:L73"/>
-    <mergeCell ref="L76:L77"/>
-    <mergeCell ref="Q8:Q12"/>
-    <mergeCell ref="Q55:Q56"/>
-    <mergeCell ref="Q64:Q65"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="U62:U64"/>
+  <mergeCells count="85">
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="U63:U65"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
@@ -5555,12 +5504,79 @@
     <mergeCell ref="M1:N1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="C46:C47"/>
+    <mergeCell ref="C47:C48"/>
     <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K31:K32"/>
-    <mergeCell ref="K46:K47"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="K47:K48"/>
     <mergeCell ref="Q3:Q7"/>
     <mergeCell ref="R3:R7"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="L73:L74"/>
+    <mergeCell ref="L77:L78"/>
+    <mergeCell ref="Q8:Q12"/>
+    <mergeCell ref="Q56:Q57"/>
+    <mergeCell ref="Q65:Q66"/>
+    <mergeCell ref="R65:R66"/>
+    <mergeCell ref="K77:K78"/>
+    <mergeCell ref="K73:K74"/>
+    <mergeCell ref="T60:T61"/>
+    <mergeCell ref="T65:T67"/>
+    <mergeCell ref="T63:T64"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="T29:T30"/>
+    <mergeCell ref="T57:T59"/>
+    <mergeCell ref="R8:R12"/>
+    <mergeCell ref="R56:R57"/>
+    <mergeCell ref="U66:U69"/>
+    <mergeCell ref="T43:T46"/>
+    <mergeCell ref="U16:U25"/>
+    <mergeCell ref="U3:U15"/>
+    <mergeCell ref="T31:T36"/>
+    <mergeCell ref="T38:T40"/>
+    <mergeCell ref="T41:T42"/>
+    <mergeCell ref="T48:T49"/>
+    <mergeCell ref="T52:T54"/>
+    <mergeCell ref="U29:U42"/>
+    <mergeCell ref="U43:U50"/>
+    <mergeCell ref="U52:U54"/>
+    <mergeCell ref="U57:U62"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="T8:T10"/>
+    <mergeCell ref="T16:T17"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B86:J86"/>
+    <mergeCell ref="H87:L87"/>
+    <mergeCell ref="H88:N88"/>
+    <mergeCell ref="J89:R89"/>
+    <mergeCell ref="J90:N90"/>
+    <mergeCell ref="N91:R91"/>
+    <mergeCell ref="N92:R92"/>
+    <mergeCell ref="P93:R93"/>
+    <mergeCell ref="P94:R94"/>
+    <mergeCell ref="P95:R95"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B100:H100"/>
+    <mergeCell ref="B101:H101"/>
+    <mergeCell ref="N110:R110"/>
+    <mergeCell ref="N111:R111"/>
+    <mergeCell ref="P112:R112"/>
+    <mergeCell ref="P113:R113"/>
+    <mergeCell ref="D102:H102"/>
+    <mergeCell ref="P114:R114"/>
+    <mergeCell ref="J107:N107"/>
+    <mergeCell ref="J106:R106"/>
+    <mergeCell ref="H105:N105"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="J108:L108"/>
+    <mergeCell ref="J109:N109"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Finish Dark Age Policies
</commit_message>
<xml_diff>
--- a/文档/政策.xlsx
+++ b/文档/政策.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Admin\Documents\GitHub\Sistine_civ6mod\文档\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E78831C-C337-447F-8BE6-5FD95DB3B6C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A859DC3-E1E2-45A8-8C77-272337DB2BAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4155" yWindow="0" windowWidth="29475" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="原版" sheetId="1" r:id="rId1"/>
@@ -1523,14 +1523,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>城市+40%产能，但城市-1宜居-5忠诚</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>有剧院广场的城市+30%锤金和+3外交支持，但这些城市-10%瓶琴</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>民主兵工厂</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1579,28 +1571,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>工业区相邻加成翻倍，所有城市+2住房，农田+1食物，伟人获取-50%（不变）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>生产开拓者+30%生产力</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <r>
-      <t>单位受伤时战斗力不下降，</t>
+      <t>单位+100%经</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
-      <t>维护费+1</t>
+      <t>验值，维护费+1</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>工业区相邻加成翻倍，所有城市+2住房，农田+1食物，伟人获取-50%（不变）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>生产开拓者+30%生产力</t>
+    <t>每个人口+2产能，但城市-1宜居-5忠诚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有剧院广场的城市+4宜居度，广播中心+3外交支持，但所有城市-20%瓶琴</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1608,7 +1607,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1634,6 +1633,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -1714,16 +1720,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3222,11 +3228,11 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L36:L37"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
     <mergeCell ref="C36:C37"/>
@@ -3237,11 +3243,11 @@
     <mergeCell ref="I34:I35"/>
     <mergeCell ref="K1:L1"/>
     <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L36:L37"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="D74:D75"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3253,8 +3259,8 @@
   <dimension ref="A1:U114"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E41" sqref="E41"/>
+      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O95" sqref="O95:R95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3372,7 +3378,7 @@
       <c r="Q3" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="R3" s="13" t="s">
         <v>369</v>
       </c>
       <c r="T3" s="12" t="s">
@@ -3420,10 +3426,10 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="L5" s="10" t="s">
         <v>418</v>
-      </c>
-      <c r="L5" s="10" t="s">
-        <v>420</v>
       </c>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -3448,10 +3454,10 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-      <c r="K6" s="15" t="s">
+      <c r="K6" s="16" t="s">
         <v>255</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="15" t="s">
         <v>332</v>
       </c>
       <c r="M6" s="5"/>
@@ -3480,8 +3486,8 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
@@ -3684,7 +3690,7 @@
         <v>42</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
@@ -3785,7 +3791,7 @@
       <c r="Q16" s="5"/>
       <c r="R16" s="5"/>
       <c r="T16" s="12" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="U16" s="12" t="s">
         <v>308</v>
@@ -3835,10 +3841,10 @@
       <c r="I18" s="5"/>
       <c r="J18" s="6"/>
       <c r="K18" s="10" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="5"/>
@@ -3847,7 +3853,7 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="5"/>
       <c r="T18" s="3" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="U18" s="12"/>
     </row>
@@ -4100,10 +4106,10 @@
       <c r="H29" s="5"/>
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
-      <c r="K29" s="13" t="s">
+      <c r="K29" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="L29" s="13" t="s">
+      <c r="L29" s="15" t="s">
         <v>407</v>
       </c>
       <c r="M29" s="5"/>
@@ -4134,8 +4140,8 @@
       <c r="H30" s="5"/>
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
       <c r="M30" s="5"/>
       <c r="N30" s="5"/>
       <c r="O30" s="5"/>
@@ -4405,7 +4411,7 @@
         <v>116</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
@@ -4415,7 +4421,7 @@
         <v>118</v>
       </c>
       <c r="J40" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="T40" s="11"/>
       <c r="U40" s="12"/>
@@ -4425,7 +4431,7 @@
         <v>119</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -4433,7 +4439,7 @@
       <c r="H41" s="5"/>
       <c r="I41" s="14"/>
       <c r="J41" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="T41" s="11" t="s">
         <v>280</v>
@@ -4543,10 +4549,10 @@
       </c>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
-      <c r="K47" s="15" t="s">
+      <c r="K47" s="16" t="s">
         <v>281</v>
       </c>
-      <c r="L47" s="13" t="s">
+      <c r="L47" s="15" t="s">
         <v>362</v>
       </c>
       <c r="T47" s="1" t="s">
@@ -4565,8 +4571,8 @@
       <c r="H48" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
+      <c r="K48" s="16"/>
+      <c r="L48" s="16"/>
       <c r="T48" s="11" t="s">
         <v>282</v>
       </c>
@@ -4687,7 +4693,7 @@
       <c r="Q56" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="R56" s="16" t="s">
+      <c r="R56" s="13" t="s">
         <v>377</v>
       </c>
       <c r="T56" s="1" t="s">
@@ -4935,10 +4941,10 @@
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
       <c r="K68" s="10" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="L68" s="10" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="T68" s="2" t="s">
         <v>297</v>
@@ -5012,7 +5018,7 @@
       <c r="C74" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="D74" s="16" t="s">
+      <c r="D74" s="13" t="s">
         <v>314</v>
       </c>
       <c r="E74" s="5"/>
@@ -5121,165 +5127,165 @@
       <c r="A83" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="13" t="s">
         <v>401</v>
       </c>
-      <c r="C83" s="16"/>
-      <c r="D83" s="16"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
+      <c r="C83" s="13"/>
+      <c r="D83" s="13"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
     </row>
     <row r="84" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A84" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="B84" s="16" t="s">
-        <v>423</v>
-      </c>
-      <c r="C84" s="16"/>
-      <c r="D84" s="16"/>
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="16"/>
-      <c r="H84" s="16"/>
+      <c r="B84" s="13" t="s">
+        <v>421</v>
+      </c>
+      <c r="C84" s="13"/>
+      <c r="D84" s="13"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
     </row>
     <row r="85" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A85" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="13" t="s">
         <v>402</v>
       </c>
-      <c r="C85" s="16"/>
-      <c r="D85" s="16"/>
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="16"/>
-      <c r="H85" s="16"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
     </row>
     <row r="86" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A86" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="13" t="s">
         <v>399</v>
       </c>
-      <c r="C86" s="16"/>
-      <c r="D86" s="16"/>
-      <c r="E86" s="16"/>
-      <c r="F86" s="16"/>
-      <c r="G86" s="16"/>
-      <c r="H86" s="16"/>
-      <c r="I86" s="16"/>
-      <c r="J86" s="16"/>
+      <c r="C86" s="13"/>
+      <c r="D86" s="13"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
     </row>
     <row r="87" spans="1:18" ht="67.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G87" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="H87" s="16" t="s">
-        <v>422</v>
-      </c>
-      <c r="I87" s="16"/>
-      <c r="J87" s="16"/>
-      <c r="K87" s="16"/>
-      <c r="L87" s="16"/>
+      <c r="H87" s="13" t="s">
+        <v>420</v>
+      </c>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="13"/>
+      <c r="L87" s="13"/>
     </row>
     <row r="88" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G88" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="H88" s="16" t="s">
+      <c r="H88" s="13" t="s">
         <v>400</v>
       </c>
-      <c r="I88" s="16"/>
-      <c r="J88" s="16"/>
-      <c r="K88" s="16"/>
-      <c r="L88" s="16"/>
-      <c r="M88" s="16"/>
-      <c r="N88" s="16"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="13"/>
+      <c r="L88" s="13"/>
+      <c r="M88" s="13"/>
+      <c r="N88" s="13"/>
     </row>
     <row r="89" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="I89" s="3" t="s">
+      <c r="I89" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="J89" s="12" t="s">
+      <c r="J89" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="K89" s="12"/>
-      <c r="L89" s="12"/>
-      <c r="M89" s="12"/>
-      <c r="N89" s="12"/>
-      <c r="O89" s="12"/>
-      <c r="P89" s="12"/>
-      <c r="Q89" s="12"/>
-      <c r="R89" s="12"/>
+      <c r="K89" s="13"/>
+      <c r="L89" s="13"/>
+      <c r="M89" s="13"/>
+      <c r="N89" s="13"/>
+      <c r="O89" s="13"/>
+      <c r="P89" s="13"/>
+      <c r="Q89" s="13"/>
+      <c r="R89" s="13"/>
     </row>
     <row r="90" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I90" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="J90" s="16" t="s">
-        <v>425</v>
-      </c>
-      <c r="K90" s="16"/>
-      <c r="L90" s="16"/>
-      <c r="M90" s="16"/>
-      <c r="N90" s="16"/>
+      <c r="J90" s="13" t="s">
+        <v>422</v>
+      </c>
+      <c r="K90" s="13"/>
+      <c r="L90" s="13"/>
+      <c r="M90" s="13"/>
+      <c r="N90" s="13"/>
     </row>
     <row r="91" spans="1:18" ht="27" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M91" s="3" t="s">
+      <c r="M91" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="N91" s="12" t="s">
+      <c r="N91" s="13" t="s">
         <v>403</v>
       </c>
-      <c r="O91" s="12"/>
-      <c r="P91" s="12"/>
-      <c r="Q91" s="12"/>
-      <c r="R91" s="12"/>
+      <c r="O91" s="13"/>
+      <c r="P91" s="13"/>
+      <c r="Q91" s="13"/>
+      <c r="R91" s="13"/>
     </row>
     <row r="92" spans="1:18" ht="54" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="M92" s="3" t="s">
+      <c r="M92" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="N92" s="12" t="s">
+      <c r="N92" s="13" t="s">
         <v>345</v>
       </c>
-      <c r="O92" s="12"/>
-      <c r="P92" s="12"/>
-      <c r="Q92" s="12"/>
-      <c r="R92" s="12"/>
+      <c r="O92" s="13"/>
+      <c r="P92" s="13"/>
+      <c r="Q92" s="13"/>
+      <c r="R92" s="13"/>
     </row>
     <row r="93" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O93" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="P93" s="16" t="s">
+      <c r="P93" s="13" t="s">
         <v>347</v>
       </c>
-      <c r="Q93" s="16"/>
-      <c r="R93" s="16"/>
+      <c r="Q93" s="13"/>
+      <c r="R93" s="13"/>
     </row>
     <row r="94" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O94" s="3" t="s">
+      <c r="O94" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="P94" s="12" t="s">
-        <v>410</v>
-      </c>
-      <c r="Q94" s="12"/>
-      <c r="R94" s="12"/>
+      <c r="P94" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="Q94" s="13"/>
+      <c r="R94" s="13"/>
     </row>
     <row r="95" spans="1:18" ht="40.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="O95" s="3" t="s">
+      <c r="O95" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="P95" s="12" t="s">
-        <v>411</v>
-      </c>
-      <c r="Q95" s="12"/>
-      <c r="R95" s="12"/>
+      <c r="P95" s="13" t="s">
+        <v>426</v>
+      </c>
+      <c r="Q95" s="13"/>
+      <c r="R95" s="13"/>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A97" s="3" t="s">
@@ -5496,34 +5502,47 @@
     </row>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="P114:R114"/>
-    <mergeCell ref="J107:N107"/>
-    <mergeCell ref="J106:R106"/>
-    <mergeCell ref="H105:N105"/>
-    <mergeCell ref="H103:L103"/>
-    <mergeCell ref="J108:L108"/>
-    <mergeCell ref="J109:N109"/>
-    <mergeCell ref="B101:H101"/>
-    <mergeCell ref="N110:R110"/>
-    <mergeCell ref="N111:R111"/>
-    <mergeCell ref="P112:R112"/>
-    <mergeCell ref="P113:R113"/>
-    <mergeCell ref="D102:H102"/>
-    <mergeCell ref="P93:R93"/>
-    <mergeCell ref="P94:R94"/>
-    <mergeCell ref="P95:R95"/>
-    <mergeCell ref="B98:F98"/>
-    <mergeCell ref="B100:H100"/>
-    <mergeCell ref="H88:N88"/>
-    <mergeCell ref="J89:R89"/>
-    <mergeCell ref="J90:N90"/>
-    <mergeCell ref="N91:R91"/>
-    <mergeCell ref="N92:R92"/>
-    <mergeCell ref="B83:F83"/>
-    <mergeCell ref="B84:H84"/>
-    <mergeCell ref="B85:H85"/>
-    <mergeCell ref="B86:J86"/>
-    <mergeCell ref="H87:L87"/>
+    <mergeCell ref="U63:U65"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K32:K33"/>
+    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="L47:L48"/>
+    <mergeCell ref="L73:L74"/>
+    <mergeCell ref="K29:K30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="C74:C75"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I40:I41"/>
+    <mergeCell ref="Q8:Q12"/>
+    <mergeCell ref="Q56:Q57"/>
+    <mergeCell ref="Q65:Q66"/>
+    <mergeCell ref="R65:R66"/>
+    <mergeCell ref="Q3:Q7"/>
+    <mergeCell ref="R3:R7"/>
+    <mergeCell ref="K77:K78"/>
+    <mergeCell ref="K73:K74"/>
+    <mergeCell ref="T60:T61"/>
+    <mergeCell ref="T65:T67"/>
+    <mergeCell ref="T63:T64"/>
+    <mergeCell ref="L77:L78"/>
+    <mergeCell ref="T24:T25"/>
+    <mergeCell ref="T29:T30"/>
+    <mergeCell ref="T57:T59"/>
+    <mergeCell ref="R8:R12"/>
+    <mergeCell ref="R56:R57"/>
     <mergeCell ref="U66:U69"/>
     <mergeCell ref="T43:T46"/>
     <mergeCell ref="U16:U25"/>
@@ -5540,47 +5559,34 @@
     <mergeCell ref="T3:T4"/>
     <mergeCell ref="T8:T10"/>
     <mergeCell ref="T16:T17"/>
-    <mergeCell ref="T24:T25"/>
-    <mergeCell ref="T29:T30"/>
-    <mergeCell ref="T57:T59"/>
-    <mergeCell ref="R8:R12"/>
-    <mergeCell ref="R56:R57"/>
-    <mergeCell ref="K77:K78"/>
-    <mergeCell ref="K73:K74"/>
-    <mergeCell ref="T60:T61"/>
-    <mergeCell ref="T65:T67"/>
-    <mergeCell ref="T63:T64"/>
-    <mergeCell ref="L77:L78"/>
-    <mergeCell ref="Q8:Q12"/>
-    <mergeCell ref="Q56:Q57"/>
-    <mergeCell ref="Q65:Q66"/>
-    <mergeCell ref="R65:R66"/>
-    <mergeCell ref="Q3:Q7"/>
-    <mergeCell ref="R3:R7"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="L47:L48"/>
-    <mergeCell ref="L73:L74"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="U63:U65"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K32:K33"/>
-    <mergeCell ref="K47:K48"/>
+    <mergeCell ref="B83:F83"/>
+    <mergeCell ref="B84:H84"/>
+    <mergeCell ref="B85:H85"/>
+    <mergeCell ref="B86:J86"/>
+    <mergeCell ref="H87:L87"/>
+    <mergeCell ref="H88:N88"/>
+    <mergeCell ref="J89:R89"/>
+    <mergeCell ref="J90:N90"/>
+    <mergeCell ref="N91:R91"/>
+    <mergeCell ref="N92:R92"/>
+    <mergeCell ref="P93:R93"/>
+    <mergeCell ref="P94:R94"/>
+    <mergeCell ref="P95:R95"/>
+    <mergeCell ref="B98:F98"/>
+    <mergeCell ref="B100:H100"/>
+    <mergeCell ref="B101:H101"/>
+    <mergeCell ref="N110:R110"/>
+    <mergeCell ref="N111:R111"/>
+    <mergeCell ref="P112:R112"/>
+    <mergeCell ref="P113:R113"/>
+    <mergeCell ref="D102:H102"/>
+    <mergeCell ref="P114:R114"/>
+    <mergeCell ref="J107:N107"/>
+    <mergeCell ref="J106:R106"/>
+    <mergeCell ref="H105:N105"/>
+    <mergeCell ref="H103:L103"/>
+    <mergeCell ref="J108:L108"/>
+    <mergeCell ref="J109:N109"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>